<commit_message>
Add esp exaples from the IoT course
</commit_message>
<xml_diff>
--- a/Documents/GanttChart_GarciaAnakabeOihanav2.xlsx
+++ b/Documents/GanttChart_GarciaAnakabeOihanav2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF52909-45E0-4C20-A05A-375F4A78B7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3B074E-52F4-44C4-949D-B1C0E2C05400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Mondragon Unibertsitatea
 TU Wien</t>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Reorganize to support SOA</t>
+  </si>
+  <si>
+    <t>Develop hardware</t>
   </si>
 </sst>
 </file>
@@ -865,8 +868,29 @@
     <xf numFmtId="14" fontId="14" fillId="2" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="3" xfId="8" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -878,29 +902,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="3" xfId="8" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1412,11 +1415,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IX35"/>
+  <dimension ref="A1:IX36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane xSplit="4" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A26" sqref="A26:D26"/>
+      <selection pane="topRight" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1454,383 +1457,383 @@
       <c r="B3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="58">
+      <c r="C3" s="70">
         <f>DATE(2021,11,3)</f>
         <v>44503</v>
       </c>
-      <c r="D3" s="58"/>
+      <c r="D3" s="70"/>
     </row>
     <row r="4" spans="1:258" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="G4" s="59">
+      <c r="G4" s="66">
         <f>G5</f>
         <v>44501</v>
       </c>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="59">
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="66">
         <f>N5</f>
         <v>44508</v>
       </c>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="60"/>
-      <c r="S4" s="60"/>
-      <c r="T4" s="61"/>
-      <c r="U4" s="59">
+      <c r="O4" s="67"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="66">
         <f>U5</f>
         <v>44515</v>
       </c>
-      <c r="V4" s="60"/>
-      <c r="W4" s="60"/>
-      <c r="X4" s="60"/>
-      <c r="Y4" s="60"/>
-      <c r="Z4" s="60"/>
-      <c r="AA4" s="61"/>
-      <c r="AB4" s="59">
+      <c r="V4" s="67"/>
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="67"/>
+      <c r="Z4" s="67"/>
+      <c r="AA4" s="68"/>
+      <c r="AB4" s="66">
         <f>AB5</f>
         <v>44522</v>
       </c>
-      <c r="AC4" s="60"/>
-      <c r="AD4" s="60"/>
-      <c r="AE4" s="60"/>
-      <c r="AF4" s="60"/>
-      <c r="AG4" s="60"/>
-      <c r="AH4" s="61"/>
-      <c r="AI4" s="59">
+      <c r="AC4" s="67"/>
+      <c r="AD4" s="67"/>
+      <c r="AE4" s="67"/>
+      <c r="AF4" s="67"/>
+      <c r="AG4" s="67"/>
+      <c r="AH4" s="68"/>
+      <c r="AI4" s="66">
         <f>AI5</f>
         <v>44529</v>
       </c>
-      <c r="AJ4" s="60"/>
-      <c r="AK4" s="60"/>
-      <c r="AL4" s="60"/>
-      <c r="AM4" s="60"/>
-      <c r="AN4" s="60"/>
-      <c r="AO4" s="61"/>
-      <c r="AP4" s="59">
+      <c r="AJ4" s="67"/>
+      <c r="AK4" s="67"/>
+      <c r="AL4" s="67"/>
+      <c r="AM4" s="67"/>
+      <c r="AN4" s="67"/>
+      <c r="AO4" s="68"/>
+      <c r="AP4" s="66">
         <f>AP5</f>
         <v>44536</v>
       </c>
-      <c r="AQ4" s="60"/>
-      <c r="AR4" s="60"/>
-      <c r="AS4" s="60"/>
-      <c r="AT4" s="60"/>
-      <c r="AU4" s="60"/>
-      <c r="AV4" s="61"/>
-      <c r="AW4" s="59">
+      <c r="AQ4" s="67"/>
+      <c r="AR4" s="67"/>
+      <c r="AS4" s="67"/>
+      <c r="AT4" s="67"/>
+      <c r="AU4" s="67"/>
+      <c r="AV4" s="68"/>
+      <c r="AW4" s="66">
         <f>AW5</f>
         <v>44543</v>
       </c>
-      <c r="AX4" s="60"/>
-      <c r="AY4" s="60"/>
-      <c r="AZ4" s="60"/>
-      <c r="BA4" s="60"/>
-      <c r="BB4" s="60"/>
-      <c r="BC4" s="61"/>
-      <c r="BD4" s="59">
+      <c r="AX4" s="67"/>
+      <c r="AY4" s="67"/>
+      <c r="AZ4" s="67"/>
+      <c r="BA4" s="67"/>
+      <c r="BB4" s="67"/>
+      <c r="BC4" s="68"/>
+      <c r="BD4" s="66">
         <f>BD5</f>
         <v>44550</v>
       </c>
-      <c r="BE4" s="60"/>
-      <c r="BF4" s="60"/>
-      <c r="BG4" s="60"/>
-      <c r="BH4" s="60"/>
-      <c r="BI4" s="60"/>
-      <c r="BJ4" s="61"/>
-      <c r="BK4" s="59">
+      <c r="BE4" s="67"/>
+      <c r="BF4" s="67"/>
+      <c r="BG4" s="67"/>
+      <c r="BH4" s="67"/>
+      <c r="BI4" s="67"/>
+      <c r="BJ4" s="68"/>
+      <c r="BK4" s="66">
         <f>BK5</f>
         <v>44557</v>
       </c>
-      <c r="BL4" s="60"/>
-      <c r="BM4" s="60"/>
-      <c r="BN4" s="60"/>
-      <c r="BO4" s="60"/>
-      <c r="BP4" s="60"/>
-      <c r="BQ4" s="61"/>
-      <c r="BR4" s="59">
+      <c r="BL4" s="67"/>
+      <c r="BM4" s="67"/>
+      <c r="BN4" s="67"/>
+      <c r="BO4" s="67"/>
+      <c r="BP4" s="67"/>
+      <c r="BQ4" s="68"/>
+      <c r="BR4" s="66">
         <f>BR5</f>
         <v>44564</v>
       </c>
-      <c r="BS4" s="60"/>
-      <c r="BT4" s="60"/>
-      <c r="BU4" s="60"/>
-      <c r="BV4" s="60"/>
-      <c r="BW4" s="60"/>
-      <c r="BX4" s="61"/>
-      <c r="BY4" s="59">
+      <c r="BS4" s="67"/>
+      <c r="BT4" s="67"/>
+      <c r="BU4" s="67"/>
+      <c r="BV4" s="67"/>
+      <c r="BW4" s="67"/>
+      <c r="BX4" s="68"/>
+      <c r="BY4" s="66">
         <f>BY5</f>
         <v>44571</v>
       </c>
-      <c r="BZ4" s="60"/>
-      <c r="CA4" s="60"/>
-      <c r="CB4" s="60"/>
-      <c r="CC4" s="60"/>
-      <c r="CD4" s="60"/>
-      <c r="CE4" s="61"/>
-      <c r="CF4" s="59">
+      <c r="BZ4" s="67"/>
+      <c r="CA4" s="67"/>
+      <c r="CB4" s="67"/>
+      <c r="CC4" s="67"/>
+      <c r="CD4" s="67"/>
+      <c r="CE4" s="68"/>
+      <c r="CF4" s="66">
         <f>CF5</f>
         <v>44578</v>
       </c>
-      <c r="CG4" s="60"/>
-      <c r="CH4" s="60"/>
-      <c r="CI4" s="60"/>
-      <c r="CJ4" s="60"/>
-      <c r="CK4" s="60"/>
-      <c r="CL4" s="61"/>
-      <c r="CM4" s="59">
+      <c r="CG4" s="67"/>
+      <c r="CH4" s="67"/>
+      <c r="CI4" s="67"/>
+      <c r="CJ4" s="67"/>
+      <c r="CK4" s="67"/>
+      <c r="CL4" s="68"/>
+      <c r="CM4" s="66">
         <f>CM5</f>
         <v>44585</v>
       </c>
-      <c r="CN4" s="60"/>
-      <c r="CO4" s="60"/>
-      <c r="CP4" s="60"/>
-      <c r="CQ4" s="60"/>
-      <c r="CR4" s="60"/>
-      <c r="CS4" s="61"/>
-      <c r="CT4" s="59">
+      <c r="CN4" s="67"/>
+      <c r="CO4" s="67"/>
+      <c r="CP4" s="67"/>
+      <c r="CQ4" s="67"/>
+      <c r="CR4" s="67"/>
+      <c r="CS4" s="68"/>
+      <c r="CT4" s="66">
         <f>CT5</f>
         <v>44592</v>
       </c>
-      <c r="CU4" s="60"/>
-      <c r="CV4" s="60"/>
-      <c r="CW4" s="60"/>
-      <c r="CX4" s="60"/>
-      <c r="CY4" s="60"/>
-      <c r="CZ4" s="61"/>
-      <c r="DA4" s="59">
+      <c r="CU4" s="67"/>
+      <c r="CV4" s="67"/>
+      <c r="CW4" s="67"/>
+      <c r="CX4" s="67"/>
+      <c r="CY4" s="67"/>
+      <c r="CZ4" s="68"/>
+      <c r="DA4" s="66">
         <f>DA5</f>
         <v>44599</v>
       </c>
-      <c r="DB4" s="60"/>
-      <c r="DC4" s="60"/>
-      <c r="DD4" s="60"/>
-      <c r="DE4" s="60"/>
-      <c r="DF4" s="60"/>
-      <c r="DG4" s="61"/>
-      <c r="DH4" s="59">
+      <c r="DB4" s="67"/>
+      <c r="DC4" s="67"/>
+      <c r="DD4" s="67"/>
+      <c r="DE4" s="67"/>
+      <c r="DF4" s="67"/>
+      <c r="DG4" s="68"/>
+      <c r="DH4" s="66">
         <f>DH5</f>
         <v>44606</v>
       </c>
-      <c r="DI4" s="60"/>
-      <c r="DJ4" s="60"/>
-      <c r="DK4" s="60"/>
-      <c r="DL4" s="60"/>
-      <c r="DM4" s="60"/>
-      <c r="DN4" s="61"/>
-      <c r="DO4" s="59">
+      <c r="DI4" s="67"/>
+      <c r="DJ4" s="67"/>
+      <c r="DK4" s="67"/>
+      <c r="DL4" s="67"/>
+      <c r="DM4" s="67"/>
+      <c r="DN4" s="68"/>
+      <c r="DO4" s="66">
         <f>DO5</f>
         <v>44613</v>
       </c>
-      <c r="DP4" s="60"/>
-      <c r="DQ4" s="60"/>
-      <c r="DR4" s="60"/>
-      <c r="DS4" s="60"/>
-      <c r="DT4" s="60"/>
-      <c r="DU4" s="61"/>
-      <c r="DV4" s="59">
+      <c r="DP4" s="67"/>
+      <c r="DQ4" s="67"/>
+      <c r="DR4" s="67"/>
+      <c r="DS4" s="67"/>
+      <c r="DT4" s="67"/>
+      <c r="DU4" s="68"/>
+      <c r="DV4" s="66">
         <f>DV5</f>
         <v>44620</v>
       </c>
-      <c r="DW4" s="60"/>
-      <c r="DX4" s="60"/>
-      <c r="DY4" s="60"/>
-      <c r="DZ4" s="60"/>
-      <c r="EA4" s="60"/>
-      <c r="EB4" s="61"/>
-      <c r="EC4" s="59">
+      <c r="DW4" s="67"/>
+      <c r="DX4" s="67"/>
+      <c r="DY4" s="67"/>
+      <c r="DZ4" s="67"/>
+      <c r="EA4" s="67"/>
+      <c r="EB4" s="68"/>
+      <c r="EC4" s="66">
         <f>EC5</f>
         <v>44627</v>
       </c>
-      <c r="ED4" s="60"/>
-      <c r="EE4" s="60"/>
-      <c r="EF4" s="60"/>
-      <c r="EG4" s="60"/>
-      <c r="EH4" s="60"/>
-      <c r="EI4" s="61"/>
-      <c r="EJ4" s="59">
+      <c r="ED4" s="67"/>
+      <c r="EE4" s="67"/>
+      <c r="EF4" s="67"/>
+      <c r="EG4" s="67"/>
+      <c r="EH4" s="67"/>
+      <c r="EI4" s="68"/>
+      <c r="EJ4" s="66">
         <f>EJ5</f>
         <v>44634</v>
       </c>
-      <c r="EK4" s="60"/>
-      <c r="EL4" s="60"/>
-      <c r="EM4" s="60"/>
-      <c r="EN4" s="60"/>
-      <c r="EO4" s="60"/>
-      <c r="EP4" s="61"/>
-      <c r="EQ4" s="59">
+      <c r="EK4" s="67"/>
+      <c r="EL4" s="67"/>
+      <c r="EM4" s="67"/>
+      <c r="EN4" s="67"/>
+      <c r="EO4" s="67"/>
+      <c r="EP4" s="68"/>
+      <c r="EQ4" s="66">
         <f>EQ5</f>
         <v>44641</v>
       </c>
-      <c r="ER4" s="60"/>
-      <c r="ES4" s="60"/>
-      <c r="ET4" s="60"/>
-      <c r="EU4" s="60"/>
-      <c r="EV4" s="60"/>
-      <c r="EW4" s="61"/>
-      <c r="EX4" s="59">
+      <c r="ER4" s="67"/>
+      <c r="ES4" s="67"/>
+      <c r="ET4" s="67"/>
+      <c r="EU4" s="67"/>
+      <c r="EV4" s="67"/>
+      <c r="EW4" s="68"/>
+      <c r="EX4" s="66">
         <f>EX5</f>
         <v>44648</v>
       </c>
-      <c r="EY4" s="60"/>
-      <c r="EZ4" s="60"/>
-      <c r="FA4" s="60"/>
-      <c r="FB4" s="60"/>
-      <c r="FC4" s="60"/>
-      <c r="FD4" s="61"/>
-      <c r="FE4" s="59">
+      <c r="EY4" s="67"/>
+      <c r="EZ4" s="67"/>
+      <c r="FA4" s="67"/>
+      <c r="FB4" s="67"/>
+      <c r="FC4" s="67"/>
+      <c r="FD4" s="68"/>
+      <c r="FE4" s="66">
         <f>FE5</f>
         <v>44655</v>
       </c>
-      <c r="FF4" s="60"/>
-      <c r="FG4" s="60"/>
-      <c r="FH4" s="60"/>
-      <c r="FI4" s="60"/>
-      <c r="FJ4" s="60"/>
-      <c r="FK4" s="61"/>
-      <c r="FL4" s="59">
+      <c r="FF4" s="67"/>
+      <c r="FG4" s="67"/>
+      <c r="FH4" s="67"/>
+      <c r="FI4" s="67"/>
+      <c r="FJ4" s="67"/>
+      <c r="FK4" s="68"/>
+      <c r="FL4" s="66">
         <f>FL5</f>
         <v>44662</v>
       </c>
-      <c r="FM4" s="60"/>
-      <c r="FN4" s="60"/>
-      <c r="FO4" s="60"/>
-      <c r="FP4" s="60"/>
-      <c r="FQ4" s="60"/>
-      <c r="FR4" s="61"/>
-      <c r="FS4" s="59">
+      <c r="FM4" s="67"/>
+      <c r="FN4" s="67"/>
+      <c r="FO4" s="67"/>
+      <c r="FP4" s="67"/>
+      <c r="FQ4" s="67"/>
+      <c r="FR4" s="68"/>
+      <c r="FS4" s="66">
         <f>FS5</f>
         <v>44669</v>
       </c>
-      <c r="FT4" s="60"/>
-      <c r="FU4" s="60"/>
-      <c r="FV4" s="60"/>
-      <c r="FW4" s="60"/>
-      <c r="FX4" s="60"/>
-      <c r="FY4" s="61"/>
-      <c r="FZ4" s="59">
+      <c r="FT4" s="67"/>
+      <c r="FU4" s="67"/>
+      <c r="FV4" s="67"/>
+      <c r="FW4" s="67"/>
+      <c r="FX4" s="67"/>
+      <c r="FY4" s="68"/>
+      <c r="FZ4" s="66">
         <f>FZ5</f>
         <v>44676</v>
       </c>
-      <c r="GA4" s="60"/>
-      <c r="GB4" s="60"/>
-      <c r="GC4" s="60"/>
-      <c r="GD4" s="60"/>
-      <c r="GE4" s="60"/>
-      <c r="GF4" s="61"/>
-      <c r="GG4" s="59">
+      <c r="GA4" s="67"/>
+      <c r="GB4" s="67"/>
+      <c r="GC4" s="67"/>
+      <c r="GD4" s="67"/>
+      <c r="GE4" s="67"/>
+      <c r="GF4" s="68"/>
+      <c r="GG4" s="66">
         <f>GG5</f>
         <v>44683</v>
       </c>
-      <c r="GH4" s="60"/>
-      <c r="GI4" s="60"/>
-      <c r="GJ4" s="60"/>
-      <c r="GK4" s="60"/>
-      <c r="GL4" s="60"/>
-      <c r="GM4" s="61"/>
-      <c r="GN4" s="59">
+      <c r="GH4" s="67"/>
+      <c r="GI4" s="67"/>
+      <c r="GJ4" s="67"/>
+      <c r="GK4" s="67"/>
+      <c r="GL4" s="67"/>
+      <c r="GM4" s="68"/>
+      <c r="GN4" s="66">
         <f>GN5</f>
         <v>44690</v>
       </c>
-      <c r="GO4" s="60"/>
-      <c r="GP4" s="60"/>
-      <c r="GQ4" s="60"/>
-      <c r="GR4" s="60"/>
-      <c r="GS4" s="60"/>
-      <c r="GT4" s="61"/>
-      <c r="GU4" s="59">
+      <c r="GO4" s="67"/>
+      <c r="GP4" s="67"/>
+      <c r="GQ4" s="67"/>
+      <c r="GR4" s="67"/>
+      <c r="GS4" s="67"/>
+      <c r="GT4" s="68"/>
+      <c r="GU4" s="66">
         <f>GU5</f>
         <v>44697</v>
       </c>
-      <c r="GV4" s="60"/>
-      <c r="GW4" s="60"/>
-      <c r="GX4" s="60"/>
-      <c r="GY4" s="60"/>
-      <c r="GZ4" s="60"/>
-      <c r="HA4" s="61"/>
-      <c r="HB4" s="59">
+      <c r="GV4" s="67"/>
+      <c r="GW4" s="67"/>
+      <c r="GX4" s="67"/>
+      <c r="GY4" s="67"/>
+      <c r="GZ4" s="67"/>
+      <c r="HA4" s="68"/>
+      <c r="HB4" s="66">
         <f>HB5</f>
         <v>44704</v>
       </c>
-      <c r="HC4" s="60"/>
-      <c r="HD4" s="60"/>
-      <c r="HE4" s="60"/>
-      <c r="HF4" s="60"/>
-      <c r="HG4" s="60"/>
-      <c r="HH4" s="61"/>
-      <c r="HI4" s="59">
+      <c r="HC4" s="67"/>
+      <c r="HD4" s="67"/>
+      <c r="HE4" s="67"/>
+      <c r="HF4" s="67"/>
+      <c r="HG4" s="67"/>
+      <c r="HH4" s="68"/>
+      <c r="HI4" s="66">
         <f>HI5</f>
         <v>44711</v>
       </c>
-      <c r="HJ4" s="60"/>
-      <c r="HK4" s="60"/>
-      <c r="HL4" s="60"/>
-      <c r="HM4" s="60"/>
-      <c r="HN4" s="60"/>
-      <c r="HO4" s="61"/>
-      <c r="HP4" s="59">
+      <c r="HJ4" s="67"/>
+      <c r="HK4" s="67"/>
+      <c r="HL4" s="67"/>
+      <c r="HM4" s="67"/>
+      <c r="HN4" s="67"/>
+      <c r="HO4" s="68"/>
+      <c r="HP4" s="66">
         <f>HP5</f>
         <v>44718</v>
       </c>
-      <c r="HQ4" s="60"/>
-      <c r="HR4" s="60"/>
-      <c r="HS4" s="60"/>
-      <c r="HT4" s="60"/>
-      <c r="HU4" s="60"/>
-      <c r="HV4" s="61"/>
-      <c r="HW4" s="59">
+      <c r="HQ4" s="67"/>
+      <c r="HR4" s="67"/>
+      <c r="HS4" s="67"/>
+      <c r="HT4" s="67"/>
+      <c r="HU4" s="67"/>
+      <c r="HV4" s="68"/>
+      <c r="HW4" s="66">
         <f>HW5</f>
         <v>44725</v>
       </c>
-      <c r="HX4" s="60"/>
-      <c r="HY4" s="60"/>
-      <c r="HZ4" s="60"/>
-      <c r="IA4" s="60"/>
-      <c r="IB4" s="60"/>
-      <c r="IC4" s="61"/>
-      <c r="ID4" s="59">
+      <c r="HX4" s="67"/>
+      <c r="HY4" s="67"/>
+      <c r="HZ4" s="67"/>
+      <c r="IA4" s="67"/>
+      <c r="IB4" s="67"/>
+      <c r="IC4" s="68"/>
+      <c r="ID4" s="66">
         <f>ID5</f>
         <v>44732</v>
       </c>
-      <c r="IE4" s="60"/>
-      <c r="IF4" s="60"/>
-      <c r="IG4" s="60"/>
-      <c r="IH4" s="60"/>
-      <c r="II4" s="60"/>
-      <c r="IJ4" s="61"/>
-      <c r="IK4" s="59">
+      <c r="IE4" s="67"/>
+      <c r="IF4" s="67"/>
+      <c r="IG4" s="67"/>
+      <c r="IH4" s="67"/>
+      <c r="II4" s="67"/>
+      <c r="IJ4" s="68"/>
+      <c r="IK4" s="66">
         <f>IK5</f>
         <v>44739</v>
       </c>
-      <c r="IL4" s="60"/>
-      <c r="IM4" s="60"/>
-      <c r="IN4" s="60"/>
-      <c r="IO4" s="60"/>
-      <c r="IP4" s="60"/>
-      <c r="IQ4" s="61"/>
-      <c r="IR4" s="59">
+      <c r="IL4" s="67"/>
+      <c r="IM4" s="67"/>
+      <c r="IN4" s="67"/>
+      <c r="IO4" s="67"/>
+      <c r="IP4" s="67"/>
+      <c r="IQ4" s="68"/>
+      <c r="IR4" s="66">
         <f>IR5</f>
         <v>44746</v>
       </c>
-      <c r="IS4" s="60"/>
-      <c r="IT4" s="60"/>
-      <c r="IU4" s="60"/>
-      <c r="IV4" s="60"/>
-      <c r="IW4" s="60"/>
-      <c r="IX4" s="61"/>
+      <c r="IS4" s="67"/>
+      <c r="IT4" s="67"/>
+      <c r="IU4" s="67"/>
+      <c r="IV4" s="67"/>
+      <c r="IW4" s="67"/>
+      <c r="IX4" s="68"/>
     </row>
     <row r="5" spans="1:258" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="62"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
       <c r="G5" s="9">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44501</v>
@@ -4124,10 +4127,10 @@
       <c r="IX7" s="14"/>
     </row>
     <row r="8" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="69"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="43" t="s">
         <v>29</v>
       </c>
@@ -4136,7 +4139,7 @@
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13">
-        <f t="shared" ref="F8:F33" si="156">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="F8:F34" si="156">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>41</v>
       </c>
       <c r="G8" s="14"/>
@@ -4393,10 +4396,10 @@
       <c r="IX8" s="14"/>
     </row>
     <row r="9" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="65"/>
+      <c r="B9" s="60"/>
       <c r="C9" s="34">
         <f>Project_Start</f>
         <v>44503</v>
@@ -4664,10 +4667,10 @@
       <c r="IX9" s="14"/>
     </row>
     <row r="10" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="66"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="24">
         <f>D9+1</f>
         <v>44513</v>
@@ -4935,10 +4938,10 @@
       <c r="IX10" s="14"/>
     </row>
     <row r="11" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="66"/>
+      <c r="B11" s="58"/>
       <c r="C11" s="24">
         <f>DATE(2021,11,24)</f>
         <v>44524</v>
@@ -5206,10 +5209,10 @@
       <c r="IX11" s="14"/>
     </row>
     <row r="12" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="67"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="35">
         <f>DATE(2021,11,31)</f>
         <v>44531</v>
@@ -5477,10 +5480,10 @@
       <c r="IX12" s="14"/>
     </row>
     <row r="13" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="64"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="45" t="s">
         <v>31</v>
       </c>
@@ -5747,10 +5750,10 @@
       <c r="IX13" s="14"/>
     </row>
     <row r="14" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="65"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="34">
         <f>DATE(2021,11,19)</f>
         <v>44519</v>
@@ -6018,10 +6021,10 @@
       <c r="IX14" s="14"/>
     </row>
     <row r="15" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="66"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="24">
         <f>DATE(2022,1,10)</f>
         <v>44571</v>
@@ -6289,10 +6292,10 @@
       <c r="IX15" s="14"/>
     </row>
     <row r="16" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="67"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="35">
         <f>DATE(2022,2,7)</f>
         <v>44599</v>
@@ -6560,16 +6563,16 @@
       <c r="IX16" s="14"/>
     </row>
     <row r="17" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="64"/>
+      <c r="B17" s="65"/>
       <c r="C17" s="36" t="str">
         <f>C18</f>
         <v>14/12/2021</v>
       </c>
       <c r="D17" s="37">
-        <f>D27</f>
+        <f>D28</f>
         <v>44742</v>
       </c>
       <c r="E17" s="13"/>
@@ -6831,21 +6834,21 @@
       <c r="IX17" s="14"/>
     </row>
     <row r="18" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="65"/>
+      <c r="B18" s="60"/>
       <c r="C18" s="46" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="38">
-        <f>DATE(2022,4,1)</f>
-        <v>44652</v>
+        <f>DATE(2022,4,3)</f>
+        <v>44654</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13">
         <f t="shared" si="156"/>
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
@@ -8712,17 +8715,17 @@
       <c r="IX24" s="14"/>
     </row>
     <row r="25" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="56"/>
-      <c r="C25" s="57">
-        <f>DATE(2022,4,1)</f>
-        <v>44652</v>
-      </c>
-      <c r="D25" s="57">
-        <f>DATE(2022,6,30)</f>
-        <v>44742</v>
+      <c r="A25" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="32"/>
+      <c r="C25" s="33">
+        <f>DATE(2022,3,29)</f>
+        <v>44649</v>
+      </c>
+      <c r="D25" s="33">
+        <f>DATE(2022,4,4)</f>
+        <v>44655</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
@@ -8980,10 +8983,18 @@
       <c r="IX25" s="14"/>
     </row>
     <row r="26" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="31"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
+      <c r="A26" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="56"/>
+      <c r="C26" s="57">
+        <f>DATE(2022,4,4)</f>
+        <v>44655</v>
+      </c>
+      <c r="D26" s="57">
+        <f>DATE(2022,6,30)</f>
+        <v>44742</v>
+      </c>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="14"/>
@@ -9240,18 +9251,10 @@
       <c r="IX26" s="14"/>
     </row>
     <row r="27" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="66"/>
-      <c r="C27" s="24">
-        <f>DATE(2022,2,21)</f>
-        <v>44613</v>
-      </c>
-      <c r="D27" s="24">
-        <f>DATE(2022,6,30)</f>
-        <v>44742</v>
-      </c>
+      <c r="A27" s="31"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="14"/>
@@ -9508,23 +9511,20 @@
       <c r="IX27" s="14"/>
     </row>
     <row r="28" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="67"/>
-      <c r="C28" s="35">
-        <f>DATE(2022,1,1)</f>
-        <v>44562</v>
-      </c>
-      <c r="D28" s="35">
-        <f>DATE(2022,1,23)</f>
-        <v>44584</v>
+      <c r="A28" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="58"/>
+      <c r="C28" s="24">
+        <f>DATE(2022,2,21)</f>
+        <v>44613</v>
+      </c>
+      <c r="D28" s="24">
+        <f>DATE(2022,6,30)</f>
+        <v>44742</v>
       </c>
       <c r="E28" s="13"/>
-      <c r="F28" s="13">
-        <f t="shared" si="156"/>
-        <v>23</v>
-      </c>
+      <c r="F28" s="13"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
@@ -9539,235 +9539,235 @@
       <c r="R28" s="14"/>
       <c r="S28" s="14"/>
       <c r="T28" s="14"/>
-      <c r="U28" s="41"/>
-      <c r="V28" s="41"/>
-      <c r="W28" s="41"/>
-      <c r="X28" s="41"/>
-      <c r="Y28" s="41"/>
-      <c r="Z28" s="41"/>
-      <c r="AA28" s="41"/>
-      <c r="AB28" s="41"/>
-      <c r="AC28" s="41"/>
-      <c r="AD28" s="41"/>
-      <c r="AE28" s="41"/>
-      <c r="AF28" s="41"/>
-      <c r="AG28" s="41"/>
-      <c r="AH28" s="41"/>
-      <c r="AI28" s="41"/>
-      <c r="AJ28" s="41"/>
-      <c r="AK28" s="41"/>
-      <c r="AL28" s="41"/>
-      <c r="AM28" s="41"/>
-      <c r="AN28" s="41"/>
-      <c r="AO28" s="41"/>
-      <c r="AP28" s="41"/>
-      <c r="AQ28" s="41"/>
-      <c r="AR28" s="41"/>
-      <c r="AS28" s="41"/>
-      <c r="AT28" s="41"/>
-      <c r="AU28" s="41"/>
-      <c r="AV28" s="41"/>
-      <c r="AW28" s="41"/>
-      <c r="AX28" s="41"/>
-      <c r="AY28" s="41"/>
-      <c r="AZ28" s="41"/>
-      <c r="BA28" s="41"/>
-      <c r="BB28" s="41"/>
-      <c r="BC28" s="41"/>
-      <c r="BD28" s="41"/>
-      <c r="BE28" s="41"/>
-      <c r="BF28" s="41"/>
-      <c r="BG28" s="41"/>
-      <c r="BH28" s="41"/>
-      <c r="BI28" s="41"/>
-      <c r="BJ28" s="41"/>
-      <c r="BK28" s="41"/>
-      <c r="BL28" s="41"/>
-      <c r="BM28" s="41"/>
-      <c r="BN28" s="41"/>
-      <c r="BO28" s="41"/>
-      <c r="BP28" s="41"/>
-      <c r="BQ28" s="41"/>
-      <c r="BR28" s="41"/>
-      <c r="BS28" s="41"/>
-      <c r="BT28" s="41"/>
-      <c r="BU28" s="41"/>
-      <c r="BV28" s="41"/>
-      <c r="BW28" s="41"/>
-      <c r="BX28" s="41"/>
-      <c r="BY28" s="41"/>
-      <c r="BZ28" s="41"/>
-      <c r="CA28" s="41"/>
-      <c r="CB28" s="41"/>
-      <c r="CC28" s="41"/>
-      <c r="CD28" s="41"/>
-      <c r="CE28" s="41"/>
-      <c r="CF28" s="41"/>
-      <c r="CG28" s="41"/>
-      <c r="CH28" s="41"/>
-      <c r="CI28" s="41"/>
-      <c r="CJ28" s="41"/>
-      <c r="CK28" s="41"/>
-      <c r="CL28" s="41"/>
-      <c r="CM28" s="41"/>
-      <c r="CN28" s="41"/>
-      <c r="CO28" s="41"/>
-      <c r="CP28" s="41"/>
-      <c r="CQ28" s="41"/>
-      <c r="CR28" s="41"/>
-      <c r="CS28" s="41"/>
-      <c r="CT28" s="41"/>
-      <c r="CU28" s="41"/>
-      <c r="CV28" s="41"/>
-      <c r="CW28" s="41"/>
-      <c r="CX28" s="41"/>
-      <c r="CY28" s="41"/>
-      <c r="CZ28" s="41"/>
-      <c r="DA28" s="41"/>
-      <c r="DB28" s="41"/>
-      <c r="DC28" s="41"/>
-      <c r="DD28" s="41"/>
-      <c r="DE28" s="41"/>
-      <c r="DF28" s="41"/>
-      <c r="DG28" s="41"/>
-      <c r="DH28" s="41"/>
-      <c r="DI28" s="41"/>
-      <c r="DJ28" s="41"/>
-      <c r="DK28" s="41"/>
-      <c r="DL28" s="41"/>
-      <c r="DM28" s="41"/>
-      <c r="DN28" s="41"/>
-      <c r="DO28" s="41"/>
-      <c r="DP28" s="41"/>
-      <c r="DQ28" s="41"/>
-      <c r="DR28" s="41"/>
-      <c r="DS28" s="41"/>
-      <c r="DT28" s="41"/>
-      <c r="DU28" s="41"/>
-      <c r="DV28" s="41"/>
-      <c r="DW28" s="41"/>
-      <c r="DX28" s="41"/>
-      <c r="DY28" s="41"/>
-      <c r="DZ28" s="41"/>
-      <c r="EA28" s="41"/>
-      <c r="EB28" s="41"/>
-      <c r="EC28" s="41"/>
-      <c r="ED28" s="41"/>
-      <c r="EE28" s="41"/>
-      <c r="EF28" s="41"/>
-      <c r="EG28" s="41"/>
-      <c r="EH28" s="41"/>
-      <c r="EI28" s="41"/>
-      <c r="EJ28" s="41"/>
-      <c r="EK28" s="41"/>
-      <c r="EL28" s="41"/>
-      <c r="EM28" s="41"/>
-      <c r="EN28" s="41"/>
-      <c r="EO28" s="41"/>
-      <c r="EP28" s="41"/>
-      <c r="EQ28" s="41"/>
-      <c r="ER28" s="41"/>
-      <c r="ES28" s="41"/>
-      <c r="ET28" s="41"/>
-      <c r="EU28" s="41"/>
-      <c r="EV28" s="41"/>
-      <c r="EW28" s="41"/>
-      <c r="EX28" s="41"/>
-      <c r="EY28" s="41"/>
-      <c r="EZ28" s="41"/>
-      <c r="FA28" s="41"/>
-      <c r="FB28" s="41"/>
-      <c r="FC28" s="41"/>
-      <c r="FD28" s="41"/>
-      <c r="FE28" s="41"/>
-      <c r="FF28" s="41"/>
-      <c r="FG28" s="41"/>
-      <c r="FH28" s="41"/>
-      <c r="FI28" s="41"/>
-      <c r="FJ28" s="41"/>
-      <c r="FK28" s="41"/>
-      <c r="FL28" s="41"/>
-      <c r="FM28" s="41"/>
-      <c r="FN28" s="41"/>
-      <c r="FO28" s="41"/>
-      <c r="FP28" s="41"/>
-      <c r="FQ28" s="41"/>
-      <c r="FR28" s="41"/>
-      <c r="FS28" s="41"/>
-      <c r="FT28" s="41"/>
-      <c r="FU28" s="41"/>
-      <c r="FV28" s="41"/>
-      <c r="FW28" s="41"/>
-      <c r="FX28" s="41"/>
-      <c r="FY28" s="41"/>
-      <c r="FZ28" s="41"/>
-      <c r="GA28" s="41"/>
-      <c r="GB28" s="41"/>
-      <c r="GC28" s="41"/>
-      <c r="GD28" s="41"/>
-      <c r="GE28" s="41"/>
-      <c r="GF28" s="41"/>
-      <c r="GG28" s="41"/>
-      <c r="GH28" s="41"/>
-      <c r="GI28" s="41"/>
-      <c r="GJ28" s="41"/>
-      <c r="GK28" s="41"/>
-      <c r="GL28" s="41"/>
-      <c r="GM28" s="41"/>
-      <c r="GN28" s="41"/>
-      <c r="GO28" s="41"/>
-      <c r="GP28" s="41"/>
-      <c r="GQ28" s="41"/>
-      <c r="GR28" s="41"/>
-      <c r="GS28" s="41"/>
-      <c r="GT28" s="41"/>
-      <c r="GU28" s="41"/>
-      <c r="GV28" s="41"/>
-      <c r="GW28" s="41"/>
-      <c r="GX28" s="41"/>
-      <c r="GY28" s="41"/>
-      <c r="GZ28" s="41"/>
-      <c r="HA28" s="41"/>
-      <c r="HB28" s="41"/>
-      <c r="HC28" s="41"/>
-      <c r="HD28" s="41"/>
-      <c r="HE28" s="41"/>
-      <c r="HF28" s="41"/>
-      <c r="HG28" s="41"/>
-      <c r="HH28" s="41"/>
-      <c r="HI28" s="41"/>
-      <c r="HJ28" s="41"/>
-      <c r="HK28" s="41"/>
-      <c r="HL28" s="41"/>
-      <c r="HM28" s="41"/>
-      <c r="HN28" s="41"/>
-      <c r="HO28" s="41"/>
-      <c r="HP28" s="41"/>
-      <c r="HQ28" s="41"/>
-      <c r="HR28" s="41"/>
-      <c r="HS28" s="41"/>
-      <c r="HT28" s="41"/>
-      <c r="HU28" s="41"/>
-      <c r="HV28" s="41"/>
-      <c r="HW28" s="41"/>
-      <c r="HX28" s="41"/>
-      <c r="HY28" s="41"/>
-      <c r="HZ28" s="41"/>
-      <c r="IA28" s="41"/>
-      <c r="IB28" s="41"/>
-      <c r="IC28" s="41"/>
-      <c r="ID28" s="41"/>
-      <c r="IE28" s="41"/>
-      <c r="IF28" s="41"/>
-      <c r="IG28" s="41"/>
-      <c r="IH28" s="41"/>
-      <c r="II28" s="41"/>
-      <c r="IJ28" s="41"/>
-      <c r="IK28" s="41"/>
-      <c r="IL28" s="41"/>
-      <c r="IM28" s="41"/>
-      <c r="IN28" s="41"/>
-      <c r="IO28" s="41"/>
+      <c r="U28" s="14"/>
+      <c r="V28" s="14"/>
+      <c r="W28" s="14"/>
+      <c r="X28" s="14"/>
+      <c r="Y28" s="14"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="14"/>
+      <c r="AB28" s="14"/>
+      <c r="AC28" s="14"/>
+      <c r="AD28" s="14"/>
+      <c r="AE28" s="14"/>
+      <c r="AF28" s="14"/>
+      <c r="AG28" s="14"/>
+      <c r="AH28" s="14"/>
+      <c r="AI28" s="14"/>
+      <c r="AJ28" s="14"/>
+      <c r="AK28" s="14"/>
+      <c r="AL28" s="14"/>
+      <c r="AM28" s="14"/>
+      <c r="AN28" s="14"/>
+      <c r="AO28" s="14"/>
+      <c r="AP28" s="14"/>
+      <c r="AQ28" s="14"/>
+      <c r="AR28" s="14"/>
+      <c r="AS28" s="14"/>
+      <c r="AT28" s="14"/>
+      <c r="AU28" s="14"/>
+      <c r="AV28" s="14"/>
+      <c r="AW28" s="14"/>
+      <c r="AX28" s="14"/>
+      <c r="AY28" s="14"/>
+      <c r="AZ28" s="14"/>
+      <c r="BA28" s="14"/>
+      <c r="BB28" s="14"/>
+      <c r="BC28" s="14"/>
+      <c r="BD28" s="14"/>
+      <c r="BE28" s="14"/>
+      <c r="BF28" s="14"/>
+      <c r="BG28" s="14"/>
+      <c r="BH28" s="14"/>
+      <c r="BI28" s="14"/>
+      <c r="BJ28" s="14"/>
+      <c r="BK28" s="14"/>
+      <c r="BL28" s="14"/>
+      <c r="BM28" s="14"/>
+      <c r="BN28" s="14"/>
+      <c r="BO28" s="14"/>
+      <c r="BP28" s="14"/>
+      <c r="BQ28" s="14"/>
+      <c r="BR28" s="14"/>
+      <c r="BS28" s="14"/>
+      <c r="BT28" s="14"/>
+      <c r="BU28" s="14"/>
+      <c r="BV28" s="14"/>
+      <c r="BW28" s="14"/>
+      <c r="BX28" s="14"/>
+      <c r="BY28" s="14"/>
+      <c r="BZ28" s="14"/>
+      <c r="CA28" s="14"/>
+      <c r="CB28" s="14"/>
+      <c r="CC28" s="14"/>
+      <c r="CD28" s="14"/>
+      <c r="CE28" s="14"/>
+      <c r="CF28" s="14"/>
+      <c r="CG28" s="14"/>
+      <c r="CH28" s="14"/>
+      <c r="CI28" s="14"/>
+      <c r="CJ28" s="14"/>
+      <c r="CK28" s="14"/>
+      <c r="CL28" s="14"/>
+      <c r="CM28" s="14"/>
+      <c r="CN28" s="14"/>
+      <c r="CO28" s="14"/>
+      <c r="CP28" s="14"/>
+      <c r="CQ28" s="14"/>
+      <c r="CR28" s="14"/>
+      <c r="CS28" s="14"/>
+      <c r="CT28" s="14"/>
+      <c r="CU28" s="14"/>
+      <c r="CV28" s="14"/>
+      <c r="CW28" s="14"/>
+      <c r="CX28" s="14"/>
+      <c r="CY28" s="14"/>
+      <c r="CZ28" s="14"/>
+      <c r="DA28" s="14"/>
+      <c r="DB28" s="14"/>
+      <c r="DC28" s="14"/>
+      <c r="DD28" s="14"/>
+      <c r="DE28" s="14"/>
+      <c r="DF28" s="14"/>
+      <c r="DG28" s="14"/>
+      <c r="DH28" s="14"/>
+      <c r="DI28" s="14"/>
+      <c r="DJ28" s="14"/>
+      <c r="DK28" s="14"/>
+      <c r="DL28" s="14"/>
+      <c r="DM28" s="14"/>
+      <c r="DN28" s="14"/>
+      <c r="DO28" s="14"/>
+      <c r="DP28" s="14"/>
+      <c r="DQ28" s="14"/>
+      <c r="DR28" s="14"/>
+      <c r="DS28" s="14"/>
+      <c r="DT28" s="14"/>
+      <c r="DU28" s="14"/>
+      <c r="DV28" s="14"/>
+      <c r="DW28" s="14"/>
+      <c r="DX28" s="14"/>
+      <c r="DY28" s="14"/>
+      <c r="DZ28" s="14"/>
+      <c r="EA28" s="14"/>
+      <c r="EB28" s="14"/>
+      <c r="EC28" s="14"/>
+      <c r="ED28" s="14"/>
+      <c r="EE28" s="14"/>
+      <c r="EF28" s="14"/>
+      <c r="EG28" s="14"/>
+      <c r="EH28" s="14"/>
+      <c r="EI28" s="14"/>
+      <c r="EJ28" s="14"/>
+      <c r="EK28" s="14"/>
+      <c r="EL28" s="14"/>
+      <c r="EM28" s="14"/>
+      <c r="EN28" s="14"/>
+      <c r="EO28" s="14"/>
+      <c r="EP28" s="14"/>
+      <c r="EQ28" s="14"/>
+      <c r="ER28" s="14"/>
+      <c r="ES28" s="14"/>
+      <c r="ET28" s="14"/>
+      <c r="EU28" s="14"/>
+      <c r="EV28" s="14"/>
+      <c r="EW28" s="14"/>
+      <c r="EX28" s="14"/>
+      <c r="EY28" s="14"/>
+      <c r="EZ28" s="14"/>
+      <c r="FA28" s="14"/>
+      <c r="FB28" s="14"/>
+      <c r="FC28" s="14"/>
+      <c r="FD28" s="14"/>
+      <c r="FE28" s="14"/>
+      <c r="FF28" s="14"/>
+      <c r="FG28" s="14"/>
+      <c r="FH28" s="14"/>
+      <c r="FI28" s="14"/>
+      <c r="FJ28" s="14"/>
+      <c r="FK28" s="14"/>
+      <c r="FL28" s="14"/>
+      <c r="FM28" s="14"/>
+      <c r="FN28" s="14"/>
+      <c r="FO28" s="14"/>
+      <c r="FP28" s="14"/>
+      <c r="FQ28" s="14"/>
+      <c r="FR28" s="14"/>
+      <c r="FS28" s="14"/>
+      <c r="FT28" s="14"/>
+      <c r="FU28" s="14"/>
+      <c r="FV28" s="14"/>
+      <c r="FW28" s="14"/>
+      <c r="FX28" s="14"/>
+      <c r="FY28" s="14"/>
+      <c r="FZ28" s="14"/>
+      <c r="GA28" s="14"/>
+      <c r="GB28" s="14"/>
+      <c r="GC28" s="14"/>
+      <c r="GD28" s="14"/>
+      <c r="GE28" s="14"/>
+      <c r="GF28" s="14"/>
+      <c r="GG28" s="14"/>
+      <c r="GH28" s="14"/>
+      <c r="GI28" s="14"/>
+      <c r="GJ28" s="14"/>
+      <c r="GK28" s="14"/>
+      <c r="GL28" s="14"/>
+      <c r="GM28" s="14"/>
+      <c r="GN28" s="14"/>
+      <c r="GO28" s="14"/>
+      <c r="GP28" s="14"/>
+      <c r="GQ28" s="14"/>
+      <c r="GR28" s="14"/>
+      <c r="GS28" s="14"/>
+      <c r="GT28" s="14"/>
+      <c r="GU28" s="14"/>
+      <c r="GV28" s="14"/>
+      <c r="GW28" s="14"/>
+      <c r="GX28" s="14"/>
+      <c r="GY28" s="14"/>
+      <c r="GZ28" s="14"/>
+      <c r="HA28" s="14"/>
+      <c r="HB28" s="14"/>
+      <c r="HC28" s="14"/>
+      <c r="HD28" s="14"/>
+      <c r="HE28" s="14"/>
+      <c r="HF28" s="14"/>
+      <c r="HG28" s="14"/>
+      <c r="HH28" s="14"/>
+      <c r="HI28" s="14"/>
+      <c r="HJ28" s="14"/>
+      <c r="HK28" s="14"/>
+      <c r="HL28" s="14"/>
+      <c r="HM28" s="14"/>
+      <c r="HN28" s="14"/>
+      <c r="HO28" s="14"/>
+      <c r="HP28" s="14"/>
+      <c r="HQ28" s="14"/>
+      <c r="HR28" s="14"/>
+      <c r="HS28" s="14"/>
+      <c r="HT28" s="14"/>
+      <c r="HU28" s="14"/>
+      <c r="HV28" s="14"/>
+      <c r="HW28" s="14"/>
+      <c r="HX28" s="14"/>
+      <c r="HY28" s="14"/>
+      <c r="HZ28" s="14"/>
+      <c r="IA28" s="14"/>
+      <c r="IB28" s="14"/>
+      <c r="IC28" s="14"/>
+      <c r="ID28" s="14"/>
+      <c r="IE28" s="14"/>
+      <c r="IF28" s="14"/>
+      <c r="IG28" s="14"/>
+      <c r="IH28" s="14"/>
+      <c r="II28" s="14"/>
+      <c r="IJ28" s="14"/>
+      <c r="IK28" s="14"/>
+      <c r="IL28" s="14"/>
+      <c r="IM28" s="14"/>
+      <c r="IN28" s="14"/>
+      <c r="IO28" s="14"/>
       <c r="IP28" s="14"/>
       <c r="IQ28" s="14"/>
       <c r="IR28" s="14"/>
@@ -9779,20 +9779,22 @@
       <c r="IX28" s="14"/>
     </row>
     <row r="29" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="68" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="69"/>
-      <c r="C29" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="54" t="s">
-        <v>36</v>
+      <c r="A29" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="63"/>
+      <c r="C29" s="35">
+        <f>DATE(2022,1,1)</f>
+        <v>44562</v>
+      </c>
+      <c r="D29" s="35">
+        <f>DATE(2022,1,23)</f>
+        <v>44584</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="13">
         <f t="shared" si="156"/>
-        <v>160</v>
+        <v>23</v>
       </c>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
@@ -9807,237 +9809,237 @@
       <c r="Q29" s="14"/>
       <c r="R29" s="14"/>
       <c r="S29" s="14"/>
-      <c r="T29" s="39"/>
-      <c r="U29" s="55"/>
-      <c r="V29" s="55"/>
-      <c r="W29" s="55"/>
-      <c r="X29" s="55"/>
-      <c r="Y29" s="55"/>
-      <c r="Z29" s="55"/>
-      <c r="AA29" s="55"/>
-      <c r="AB29" s="55"/>
-      <c r="AC29" s="55"/>
-      <c r="AD29" s="55"/>
-      <c r="AE29" s="55"/>
-      <c r="AF29" s="55"/>
-      <c r="AG29" s="55"/>
-      <c r="AH29" s="55"/>
-      <c r="AI29" s="55"/>
-      <c r="AJ29" s="55"/>
-      <c r="AK29" s="55"/>
-      <c r="AL29" s="55"/>
-      <c r="AM29" s="55"/>
-      <c r="AN29" s="55"/>
-      <c r="AO29" s="55"/>
-      <c r="AP29" s="55"/>
-      <c r="AQ29" s="55"/>
-      <c r="AR29" s="55"/>
-      <c r="AS29" s="55"/>
-      <c r="AT29" s="55"/>
-      <c r="AU29" s="55"/>
-      <c r="AV29" s="55"/>
-      <c r="AW29" s="55"/>
-      <c r="AX29" s="55"/>
-      <c r="AY29" s="55"/>
-      <c r="AZ29" s="55"/>
-      <c r="BA29" s="55"/>
-      <c r="BB29" s="55"/>
-      <c r="BC29" s="55"/>
-      <c r="BD29" s="55"/>
-      <c r="BE29" s="55"/>
-      <c r="BF29" s="55"/>
-      <c r="BG29" s="55"/>
-      <c r="BH29" s="55"/>
-      <c r="BI29" s="55"/>
-      <c r="BJ29" s="55"/>
-      <c r="BK29" s="55"/>
-      <c r="BL29" s="55"/>
-      <c r="BM29" s="55"/>
-      <c r="BN29" s="55"/>
-      <c r="BO29" s="55"/>
-      <c r="BP29" s="55"/>
-      <c r="BQ29" s="55"/>
-      <c r="BR29" s="55"/>
-      <c r="BS29" s="55"/>
-      <c r="BT29" s="55"/>
-      <c r="BU29" s="55"/>
-      <c r="BV29" s="55"/>
-      <c r="BW29" s="55"/>
-      <c r="BX29" s="55"/>
-      <c r="BY29" s="55"/>
-      <c r="BZ29" s="55"/>
-      <c r="CA29" s="55"/>
-      <c r="CB29" s="55"/>
-      <c r="CC29" s="55"/>
-      <c r="CD29" s="55"/>
-      <c r="CE29" s="55"/>
-      <c r="CF29" s="55"/>
-      <c r="CG29" s="55"/>
-      <c r="CH29" s="55"/>
-      <c r="CI29" s="55"/>
-      <c r="CJ29" s="55"/>
-      <c r="CK29" s="55"/>
-      <c r="CL29" s="55"/>
-      <c r="CM29" s="55"/>
-      <c r="CN29" s="55"/>
-      <c r="CO29" s="55"/>
-      <c r="CP29" s="55"/>
-      <c r="CQ29" s="55"/>
-      <c r="CR29" s="55"/>
-      <c r="CS29" s="55"/>
-      <c r="CT29" s="55"/>
-      <c r="CU29" s="55"/>
-      <c r="CV29" s="55"/>
-      <c r="CW29" s="55"/>
-      <c r="CX29" s="55"/>
-      <c r="CY29" s="55"/>
-      <c r="CZ29" s="55"/>
-      <c r="DA29" s="55"/>
-      <c r="DB29" s="55"/>
-      <c r="DC29" s="55"/>
-      <c r="DD29" s="55"/>
-      <c r="DE29" s="55"/>
-      <c r="DF29" s="55"/>
-      <c r="DG29" s="55"/>
-      <c r="DH29" s="55"/>
-      <c r="DI29" s="55"/>
-      <c r="DJ29" s="55"/>
-      <c r="DK29" s="55"/>
-      <c r="DL29" s="55"/>
-      <c r="DM29" s="55"/>
-      <c r="DN29" s="55"/>
-      <c r="DO29" s="55"/>
-      <c r="DP29" s="55"/>
-      <c r="DQ29" s="55"/>
-      <c r="DR29" s="55"/>
-      <c r="DS29" s="55"/>
-      <c r="DT29" s="55"/>
-      <c r="DU29" s="55"/>
-      <c r="DV29" s="55"/>
-      <c r="DW29" s="55"/>
-      <c r="DX29" s="55"/>
-      <c r="DY29" s="55"/>
-      <c r="DZ29" s="55"/>
-      <c r="EA29" s="55"/>
-      <c r="EB29" s="55"/>
-      <c r="EC29" s="55"/>
-      <c r="ED29" s="55"/>
-      <c r="EE29" s="55"/>
-      <c r="EF29" s="55"/>
-      <c r="EG29" s="55"/>
-      <c r="EH29" s="55"/>
-      <c r="EI29" s="55"/>
-      <c r="EJ29" s="55"/>
-      <c r="EK29" s="55"/>
-      <c r="EL29" s="55"/>
-      <c r="EM29" s="55"/>
-      <c r="EN29" s="55"/>
-      <c r="EO29" s="55"/>
-      <c r="EP29" s="55"/>
-      <c r="EQ29" s="55"/>
-      <c r="ER29" s="55"/>
-      <c r="ES29" s="55"/>
-      <c r="ET29" s="55"/>
-      <c r="EU29" s="55"/>
-      <c r="EV29" s="55"/>
-      <c r="EW29" s="55"/>
-      <c r="EX29" s="55"/>
-      <c r="EY29" s="55"/>
-      <c r="EZ29" s="55"/>
-      <c r="FA29" s="55"/>
-      <c r="FB29" s="55"/>
-      <c r="FC29" s="55"/>
-      <c r="FD29" s="55"/>
-      <c r="FE29" s="55"/>
-      <c r="FF29" s="55"/>
-      <c r="FG29" s="55"/>
-      <c r="FH29" s="55"/>
-      <c r="FI29" s="55"/>
-      <c r="FJ29" s="55"/>
-      <c r="FK29" s="55"/>
-      <c r="FL29" s="55"/>
-      <c r="FM29" s="55"/>
-      <c r="FN29" s="55"/>
-      <c r="FO29" s="55"/>
-      <c r="FP29" s="55"/>
-      <c r="FQ29" s="55"/>
-      <c r="FR29" s="55"/>
-      <c r="FS29" s="55"/>
-      <c r="FT29" s="55"/>
-      <c r="FU29" s="55"/>
-      <c r="FV29" s="55"/>
-      <c r="FW29" s="55"/>
-      <c r="FX29" s="55"/>
-      <c r="FY29" s="55"/>
-      <c r="FZ29" s="55"/>
-      <c r="GA29" s="55"/>
-      <c r="GB29" s="55"/>
-      <c r="GC29" s="55"/>
-      <c r="GD29" s="55"/>
-      <c r="GE29" s="55"/>
-      <c r="GF29" s="55"/>
-      <c r="GG29" s="55"/>
-      <c r="GH29" s="55"/>
-      <c r="GI29" s="55"/>
-      <c r="GJ29" s="55"/>
-      <c r="GK29" s="55"/>
-      <c r="GL29" s="55"/>
-      <c r="GM29" s="55"/>
-      <c r="GN29" s="55"/>
-      <c r="GO29" s="55"/>
-      <c r="GP29" s="55"/>
-      <c r="GQ29" s="55"/>
-      <c r="GR29" s="55"/>
-      <c r="GS29" s="55"/>
-      <c r="GT29" s="55"/>
-      <c r="GU29" s="55"/>
-      <c r="GV29" s="55"/>
-      <c r="GW29" s="55"/>
-      <c r="GX29" s="55"/>
-      <c r="GY29" s="55"/>
-      <c r="GZ29" s="55"/>
-      <c r="HA29" s="55"/>
-      <c r="HB29" s="55"/>
-      <c r="HC29" s="55"/>
-      <c r="HD29" s="55"/>
-      <c r="HE29" s="55"/>
-      <c r="HF29" s="55"/>
-      <c r="HG29" s="55"/>
-      <c r="HH29" s="55"/>
-      <c r="HI29" s="55"/>
-      <c r="HJ29" s="55"/>
-      <c r="HK29" s="55"/>
-      <c r="HL29" s="55"/>
-      <c r="HM29" s="55"/>
-      <c r="HN29" s="55"/>
-      <c r="HO29" s="55"/>
-      <c r="HP29" s="55"/>
-      <c r="HQ29" s="55"/>
-      <c r="HR29" s="55"/>
-      <c r="HS29" s="55"/>
-      <c r="HT29" s="55"/>
-      <c r="HU29" s="55"/>
-      <c r="HV29" s="55"/>
-      <c r="HW29" s="55"/>
-      <c r="HX29" s="55"/>
-      <c r="HY29" s="55"/>
-      <c r="HZ29" s="55"/>
-      <c r="IA29" s="55"/>
-      <c r="IB29" s="55"/>
-      <c r="IC29" s="55"/>
-      <c r="ID29" s="55"/>
-      <c r="IE29" s="55"/>
-      <c r="IF29" s="55"/>
-      <c r="IG29" s="55"/>
-      <c r="IH29" s="55"/>
-      <c r="II29" s="55"/>
-      <c r="IJ29" s="55"/>
-      <c r="IK29" s="55"/>
-      <c r="IL29" s="55"/>
-      <c r="IM29" s="55"/>
-      <c r="IN29" s="55"/>
-      <c r="IO29" s="55"/>
-      <c r="IP29" s="40"/>
+      <c r="T29" s="14"/>
+      <c r="U29" s="41"/>
+      <c r="V29" s="41"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="41"/>
+      <c r="Y29" s="41"/>
+      <c r="Z29" s="41"/>
+      <c r="AA29" s="41"/>
+      <c r="AB29" s="41"/>
+      <c r="AC29" s="41"/>
+      <c r="AD29" s="41"/>
+      <c r="AE29" s="41"/>
+      <c r="AF29" s="41"/>
+      <c r="AG29" s="41"/>
+      <c r="AH29" s="41"/>
+      <c r="AI29" s="41"/>
+      <c r="AJ29" s="41"/>
+      <c r="AK29" s="41"/>
+      <c r="AL29" s="41"/>
+      <c r="AM29" s="41"/>
+      <c r="AN29" s="41"/>
+      <c r="AO29" s="41"/>
+      <c r="AP29" s="41"/>
+      <c r="AQ29" s="41"/>
+      <c r="AR29" s="41"/>
+      <c r="AS29" s="41"/>
+      <c r="AT29" s="41"/>
+      <c r="AU29" s="41"/>
+      <c r="AV29" s="41"/>
+      <c r="AW29" s="41"/>
+      <c r="AX29" s="41"/>
+      <c r="AY29" s="41"/>
+      <c r="AZ29" s="41"/>
+      <c r="BA29" s="41"/>
+      <c r="BB29" s="41"/>
+      <c r="BC29" s="41"/>
+      <c r="BD29" s="41"/>
+      <c r="BE29" s="41"/>
+      <c r="BF29" s="41"/>
+      <c r="BG29" s="41"/>
+      <c r="BH29" s="41"/>
+      <c r="BI29" s="41"/>
+      <c r="BJ29" s="41"/>
+      <c r="BK29" s="41"/>
+      <c r="BL29" s="41"/>
+      <c r="BM29" s="41"/>
+      <c r="BN29" s="41"/>
+      <c r="BO29" s="41"/>
+      <c r="BP29" s="41"/>
+      <c r="BQ29" s="41"/>
+      <c r="BR29" s="41"/>
+      <c r="BS29" s="41"/>
+      <c r="BT29" s="41"/>
+      <c r="BU29" s="41"/>
+      <c r="BV29" s="41"/>
+      <c r="BW29" s="41"/>
+      <c r="BX29" s="41"/>
+      <c r="BY29" s="41"/>
+      <c r="BZ29" s="41"/>
+      <c r="CA29" s="41"/>
+      <c r="CB29" s="41"/>
+      <c r="CC29" s="41"/>
+      <c r="CD29" s="41"/>
+      <c r="CE29" s="41"/>
+      <c r="CF29" s="41"/>
+      <c r="CG29" s="41"/>
+      <c r="CH29" s="41"/>
+      <c r="CI29" s="41"/>
+      <c r="CJ29" s="41"/>
+      <c r="CK29" s="41"/>
+      <c r="CL29" s="41"/>
+      <c r="CM29" s="41"/>
+      <c r="CN29" s="41"/>
+      <c r="CO29" s="41"/>
+      <c r="CP29" s="41"/>
+      <c r="CQ29" s="41"/>
+      <c r="CR29" s="41"/>
+      <c r="CS29" s="41"/>
+      <c r="CT29" s="41"/>
+      <c r="CU29" s="41"/>
+      <c r="CV29" s="41"/>
+      <c r="CW29" s="41"/>
+      <c r="CX29" s="41"/>
+      <c r="CY29" s="41"/>
+      <c r="CZ29" s="41"/>
+      <c r="DA29" s="41"/>
+      <c r="DB29" s="41"/>
+      <c r="DC29" s="41"/>
+      <c r="DD29" s="41"/>
+      <c r="DE29" s="41"/>
+      <c r="DF29" s="41"/>
+      <c r="DG29" s="41"/>
+      <c r="DH29" s="41"/>
+      <c r="DI29" s="41"/>
+      <c r="DJ29" s="41"/>
+      <c r="DK29" s="41"/>
+      <c r="DL29" s="41"/>
+      <c r="DM29" s="41"/>
+      <c r="DN29" s="41"/>
+      <c r="DO29" s="41"/>
+      <c r="DP29" s="41"/>
+      <c r="DQ29" s="41"/>
+      <c r="DR29" s="41"/>
+      <c r="DS29" s="41"/>
+      <c r="DT29" s="41"/>
+      <c r="DU29" s="41"/>
+      <c r="DV29" s="41"/>
+      <c r="DW29" s="41"/>
+      <c r="DX29" s="41"/>
+      <c r="DY29" s="41"/>
+      <c r="DZ29" s="41"/>
+      <c r="EA29" s="41"/>
+      <c r="EB29" s="41"/>
+      <c r="EC29" s="41"/>
+      <c r="ED29" s="41"/>
+      <c r="EE29" s="41"/>
+      <c r="EF29" s="41"/>
+      <c r="EG29" s="41"/>
+      <c r="EH29" s="41"/>
+      <c r="EI29" s="41"/>
+      <c r="EJ29" s="41"/>
+      <c r="EK29" s="41"/>
+      <c r="EL29" s="41"/>
+      <c r="EM29" s="41"/>
+      <c r="EN29" s="41"/>
+      <c r="EO29" s="41"/>
+      <c r="EP29" s="41"/>
+      <c r="EQ29" s="41"/>
+      <c r="ER29" s="41"/>
+      <c r="ES29" s="41"/>
+      <c r="ET29" s="41"/>
+      <c r="EU29" s="41"/>
+      <c r="EV29" s="41"/>
+      <c r="EW29" s="41"/>
+      <c r="EX29" s="41"/>
+      <c r="EY29" s="41"/>
+      <c r="EZ29" s="41"/>
+      <c r="FA29" s="41"/>
+      <c r="FB29" s="41"/>
+      <c r="FC29" s="41"/>
+      <c r="FD29" s="41"/>
+      <c r="FE29" s="41"/>
+      <c r="FF29" s="41"/>
+      <c r="FG29" s="41"/>
+      <c r="FH29" s="41"/>
+      <c r="FI29" s="41"/>
+      <c r="FJ29" s="41"/>
+      <c r="FK29" s="41"/>
+      <c r="FL29" s="41"/>
+      <c r="FM29" s="41"/>
+      <c r="FN29" s="41"/>
+      <c r="FO29" s="41"/>
+      <c r="FP29" s="41"/>
+      <c r="FQ29" s="41"/>
+      <c r="FR29" s="41"/>
+      <c r="FS29" s="41"/>
+      <c r="FT29" s="41"/>
+      <c r="FU29" s="41"/>
+      <c r="FV29" s="41"/>
+      <c r="FW29" s="41"/>
+      <c r="FX29" s="41"/>
+      <c r="FY29" s="41"/>
+      <c r="FZ29" s="41"/>
+      <c r="GA29" s="41"/>
+      <c r="GB29" s="41"/>
+      <c r="GC29" s="41"/>
+      <c r="GD29" s="41"/>
+      <c r="GE29" s="41"/>
+      <c r="GF29" s="41"/>
+      <c r="GG29" s="41"/>
+      <c r="GH29" s="41"/>
+      <c r="GI29" s="41"/>
+      <c r="GJ29" s="41"/>
+      <c r="GK29" s="41"/>
+      <c r="GL29" s="41"/>
+      <c r="GM29" s="41"/>
+      <c r="GN29" s="41"/>
+      <c r="GO29" s="41"/>
+      <c r="GP29" s="41"/>
+      <c r="GQ29" s="41"/>
+      <c r="GR29" s="41"/>
+      <c r="GS29" s="41"/>
+      <c r="GT29" s="41"/>
+      <c r="GU29" s="41"/>
+      <c r="GV29" s="41"/>
+      <c r="GW29" s="41"/>
+      <c r="GX29" s="41"/>
+      <c r="GY29" s="41"/>
+      <c r="GZ29" s="41"/>
+      <c r="HA29" s="41"/>
+      <c r="HB29" s="41"/>
+      <c r="HC29" s="41"/>
+      <c r="HD29" s="41"/>
+      <c r="HE29" s="41"/>
+      <c r="HF29" s="41"/>
+      <c r="HG29" s="41"/>
+      <c r="HH29" s="41"/>
+      <c r="HI29" s="41"/>
+      <c r="HJ29" s="41"/>
+      <c r="HK29" s="41"/>
+      <c r="HL29" s="41"/>
+      <c r="HM29" s="41"/>
+      <c r="HN29" s="41"/>
+      <c r="HO29" s="41"/>
+      <c r="HP29" s="41"/>
+      <c r="HQ29" s="41"/>
+      <c r="HR29" s="41"/>
+      <c r="HS29" s="41"/>
+      <c r="HT29" s="41"/>
+      <c r="HU29" s="41"/>
+      <c r="HV29" s="41"/>
+      <c r="HW29" s="41"/>
+      <c r="HX29" s="41"/>
+      <c r="HY29" s="41"/>
+      <c r="HZ29" s="41"/>
+      <c r="IA29" s="41"/>
+      <c r="IB29" s="41"/>
+      <c r="IC29" s="41"/>
+      <c r="ID29" s="41"/>
+      <c r="IE29" s="41"/>
+      <c r="IF29" s="41"/>
+      <c r="IG29" s="41"/>
+      <c r="IH29" s="41"/>
+      <c r="II29" s="41"/>
+      <c r="IJ29" s="41"/>
+      <c r="IK29" s="41"/>
+      <c r="IL29" s="41"/>
+      <c r="IM29" s="41"/>
+      <c r="IN29" s="41"/>
+      <c r="IO29" s="41"/>
+      <c r="IP29" s="14"/>
       <c r="IQ29" s="14"/>
       <c r="IR29" s="14"/>
       <c r="IS29" s="14"/>
@@ -10048,22 +10050,20 @@
       <c r="IX29" s="14"/>
     </row>
     <row r="30" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="65" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="65"/>
-      <c r="C30" s="34">
-        <f>DATE(2022,1,23)</f>
-        <v>44584</v>
-      </c>
-      <c r="D30" s="34">
-        <f>DATE(2022,2,13)</f>
-        <v>44605</v>
+      <c r="A30" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="62"/>
+      <c r="C30" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="54" t="s">
+        <v>36</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13">
         <f t="shared" si="156"/>
-        <v>22</v>
+        <v>160</v>
       </c>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -10078,237 +10078,237 @@
       <c r="Q30" s="14"/>
       <c r="R30" s="14"/>
       <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
-      <c r="U30" s="42"/>
-      <c r="V30" s="42"/>
-      <c r="W30" s="42"/>
-      <c r="X30" s="42"/>
-      <c r="Y30" s="42"/>
-      <c r="Z30" s="42"/>
-      <c r="AA30" s="42"/>
-      <c r="AB30" s="42"/>
-      <c r="AC30" s="42"/>
-      <c r="AD30" s="42"/>
-      <c r="AE30" s="42"/>
-      <c r="AF30" s="42"/>
-      <c r="AG30" s="42"/>
-      <c r="AH30" s="42"/>
-      <c r="AI30" s="42"/>
-      <c r="AJ30" s="42"/>
-      <c r="AK30" s="42"/>
-      <c r="AL30" s="42"/>
-      <c r="AM30" s="42"/>
-      <c r="AN30" s="42"/>
-      <c r="AO30" s="42"/>
-      <c r="AP30" s="42"/>
-      <c r="AQ30" s="42"/>
-      <c r="AR30" s="42"/>
-      <c r="AS30" s="42"/>
-      <c r="AT30" s="42"/>
-      <c r="AU30" s="42"/>
-      <c r="AV30" s="42"/>
-      <c r="AW30" s="42"/>
-      <c r="AX30" s="42"/>
-      <c r="AY30" s="42"/>
-      <c r="AZ30" s="42"/>
-      <c r="BA30" s="42"/>
-      <c r="BB30" s="42"/>
-      <c r="BC30" s="42"/>
-      <c r="BD30" s="42"/>
-      <c r="BE30" s="42"/>
-      <c r="BF30" s="42"/>
-      <c r="BG30" s="42"/>
-      <c r="BH30" s="42"/>
-      <c r="BI30" s="42"/>
-      <c r="BJ30" s="42"/>
-      <c r="BK30" s="42"/>
-      <c r="BL30" s="42"/>
-      <c r="BM30" s="42"/>
-      <c r="BN30" s="42"/>
-      <c r="BO30" s="42"/>
-      <c r="BP30" s="42"/>
-      <c r="BQ30" s="42"/>
-      <c r="BR30" s="42"/>
-      <c r="BS30" s="42"/>
-      <c r="BT30" s="42"/>
-      <c r="BU30" s="42"/>
-      <c r="BV30" s="42"/>
-      <c r="BW30" s="42"/>
-      <c r="BX30" s="42"/>
-      <c r="BY30" s="42"/>
-      <c r="BZ30" s="42"/>
-      <c r="CA30" s="42"/>
-      <c r="CB30" s="42"/>
-      <c r="CC30" s="42"/>
-      <c r="CD30" s="42"/>
-      <c r="CE30" s="42"/>
-      <c r="CF30" s="42"/>
-      <c r="CG30" s="42"/>
-      <c r="CH30" s="42"/>
-      <c r="CI30" s="42"/>
-      <c r="CJ30" s="42"/>
-      <c r="CK30" s="42"/>
-      <c r="CL30" s="42"/>
-      <c r="CM30" s="42"/>
-      <c r="CN30" s="42"/>
-      <c r="CO30" s="42"/>
-      <c r="CP30" s="42"/>
-      <c r="CQ30" s="42"/>
-      <c r="CR30" s="42"/>
-      <c r="CS30" s="42"/>
-      <c r="CT30" s="42"/>
-      <c r="CU30" s="42"/>
-      <c r="CV30" s="42"/>
-      <c r="CW30" s="42"/>
-      <c r="CX30" s="42"/>
-      <c r="CY30" s="42"/>
-      <c r="CZ30" s="42"/>
-      <c r="DA30" s="42"/>
-      <c r="DB30" s="42"/>
-      <c r="DC30" s="42"/>
-      <c r="DD30" s="42"/>
-      <c r="DE30" s="42"/>
-      <c r="DF30" s="42"/>
-      <c r="DG30" s="42"/>
-      <c r="DH30" s="42"/>
-      <c r="DI30" s="42"/>
-      <c r="DJ30" s="42"/>
-      <c r="DK30" s="42"/>
-      <c r="DL30" s="42"/>
-      <c r="DM30" s="42"/>
-      <c r="DN30" s="42"/>
-      <c r="DO30" s="42"/>
-      <c r="DP30" s="42"/>
-      <c r="DQ30" s="42"/>
-      <c r="DR30" s="42"/>
-      <c r="DS30" s="42"/>
-      <c r="DT30" s="42"/>
-      <c r="DU30" s="42"/>
-      <c r="DV30" s="42"/>
-      <c r="DW30" s="42"/>
-      <c r="DX30" s="42"/>
-      <c r="DY30" s="42"/>
-      <c r="DZ30" s="42"/>
-      <c r="EA30" s="42"/>
-      <c r="EB30" s="42"/>
-      <c r="EC30" s="42"/>
-      <c r="ED30" s="42"/>
-      <c r="EE30" s="42"/>
-      <c r="EF30" s="42"/>
-      <c r="EG30" s="42"/>
-      <c r="EH30" s="42"/>
-      <c r="EI30" s="42"/>
-      <c r="EJ30" s="42"/>
-      <c r="EK30" s="42"/>
-      <c r="EL30" s="42"/>
-      <c r="EM30" s="42"/>
-      <c r="EN30" s="42"/>
-      <c r="EO30" s="42"/>
-      <c r="EP30" s="42"/>
-      <c r="EQ30" s="42"/>
-      <c r="ER30" s="42"/>
-      <c r="ES30" s="42"/>
-      <c r="ET30" s="42"/>
-      <c r="EU30" s="42"/>
-      <c r="EV30" s="42"/>
-      <c r="EW30" s="42"/>
-      <c r="EX30" s="42"/>
-      <c r="EY30" s="42"/>
-      <c r="EZ30" s="42"/>
-      <c r="FA30" s="42"/>
-      <c r="FB30" s="42"/>
-      <c r="FC30" s="42"/>
-      <c r="FD30" s="42"/>
-      <c r="FE30" s="42"/>
-      <c r="FF30" s="42"/>
-      <c r="FG30" s="42"/>
-      <c r="FH30" s="42"/>
-      <c r="FI30" s="42"/>
-      <c r="FJ30" s="42"/>
-      <c r="FK30" s="42"/>
-      <c r="FL30" s="42"/>
-      <c r="FM30" s="42"/>
-      <c r="FN30" s="42"/>
-      <c r="FO30" s="42"/>
-      <c r="FP30" s="42"/>
-      <c r="FQ30" s="42"/>
-      <c r="FR30" s="42"/>
-      <c r="FS30" s="42"/>
-      <c r="FT30" s="42"/>
-      <c r="FU30" s="42"/>
-      <c r="FV30" s="42"/>
-      <c r="FW30" s="42"/>
-      <c r="FX30" s="42"/>
-      <c r="FY30" s="42"/>
-      <c r="FZ30" s="42"/>
-      <c r="GA30" s="42"/>
-      <c r="GB30" s="42"/>
-      <c r="GC30" s="42"/>
-      <c r="GD30" s="42"/>
-      <c r="GE30" s="42"/>
-      <c r="GF30" s="42"/>
-      <c r="GG30" s="42"/>
-      <c r="GH30" s="42"/>
-      <c r="GI30" s="42"/>
-      <c r="GJ30" s="42"/>
-      <c r="GK30" s="42"/>
-      <c r="GL30" s="42"/>
-      <c r="GM30" s="42"/>
-      <c r="GN30" s="42"/>
-      <c r="GO30" s="42"/>
-      <c r="GP30" s="42"/>
-      <c r="GQ30" s="42"/>
-      <c r="GR30" s="42"/>
-      <c r="GS30" s="42"/>
-      <c r="GT30" s="42"/>
-      <c r="GU30" s="42"/>
-      <c r="GV30" s="42"/>
-      <c r="GW30" s="42"/>
-      <c r="GX30" s="42"/>
-      <c r="GY30" s="42"/>
-      <c r="GZ30" s="42"/>
-      <c r="HA30" s="42"/>
-      <c r="HB30" s="42"/>
-      <c r="HC30" s="42"/>
-      <c r="HD30" s="42"/>
-      <c r="HE30" s="42"/>
-      <c r="HF30" s="42"/>
-      <c r="HG30" s="42"/>
-      <c r="HH30" s="42"/>
-      <c r="HI30" s="42"/>
-      <c r="HJ30" s="42"/>
-      <c r="HK30" s="42"/>
-      <c r="HL30" s="42"/>
-      <c r="HM30" s="42"/>
-      <c r="HN30" s="42"/>
-      <c r="HO30" s="42"/>
-      <c r="HP30" s="42"/>
-      <c r="HQ30" s="42"/>
-      <c r="HR30" s="42"/>
-      <c r="HS30" s="42"/>
-      <c r="HT30" s="42"/>
-      <c r="HU30" s="42"/>
-      <c r="HV30" s="42"/>
-      <c r="HW30" s="42"/>
-      <c r="HX30" s="42"/>
-      <c r="HY30" s="42"/>
-      <c r="HZ30" s="42"/>
-      <c r="IA30" s="42"/>
-      <c r="IB30" s="42"/>
-      <c r="IC30" s="42"/>
-      <c r="ID30" s="42"/>
-      <c r="IE30" s="42"/>
-      <c r="IF30" s="42"/>
-      <c r="IG30" s="42"/>
-      <c r="IH30" s="42"/>
-      <c r="II30" s="42"/>
-      <c r="IJ30" s="42"/>
-      <c r="IK30" s="42"/>
-      <c r="IL30" s="42"/>
-      <c r="IM30" s="42"/>
-      <c r="IN30" s="42"/>
-      <c r="IO30" s="42"/>
-      <c r="IP30" s="14"/>
+      <c r="T30" s="39"/>
+      <c r="U30" s="55"/>
+      <c r="V30" s="55"/>
+      <c r="W30" s="55"/>
+      <c r="X30" s="55"/>
+      <c r="Y30" s="55"/>
+      <c r="Z30" s="55"/>
+      <c r="AA30" s="55"/>
+      <c r="AB30" s="55"/>
+      <c r="AC30" s="55"/>
+      <c r="AD30" s="55"/>
+      <c r="AE30" s="55"/>
+      <c r="AF30" s="55"/>
+      <c r="AG30" s="55"/>
+      <c r="AH30" s="55"/>
+      <c r="AI30" s="55"/>
+      <c r="AJ30" s="55"/>
+      <c r="AK30" s="55"/>
+      <c r="AL30" s="55"/>
+      <c r="AM30" s="55"/>
+      <c r="AN30" s="55"/>
+      <c r="AO30" s="55"/>
+      <c r="AP30" s="55"/>
+      <c r="AQ30" s="55"/>
+      <c r="AR30" s="55"/>
+      <c r="AS30" s="55"/>
+      <c r="AT30" s="55"/>
+      <c r="AU30" s="55"/>
+      <c r="AV30" s="55"/>
+      <c r="AW30" s="55"/>
+      <c r="AX30" s="55"/>
+      <c r="AY30" s="55"/>
+      <c r="AZ30" s="55"/>
+      <c r="BA30" s="55"/>
+      <c r="BB30" s="55"/>
+      <c r="BC30" s="55"/>
+      <c r="BD30" s="55"/>
+      <c r="BE30" s="55"/>
+      <c r="BF30" s="55"/>
+      <c r="BG30" s="55"/>
+      <c r="BH30" s="55"/>
+      <c r="BI30" s="55"/>
+      <c r="BJ30" s="55"/>
+      <c r="BK30" s="55"/>
+      <c r="BL30" s="55"/>
+      <c r="BM30" s="55"/>
+      <c r="BN30" s="55"/>
+      <c r="BO30" s="55"/>
+      <c r="BP30" s="55"/>
+      <c r="BQ30" s="55"/>
+      <c r="BR30" s="55"/>
+      <c r="BS30" s="55"/>
+      <c r="BT30" s="55"/>
+      <c r="BU30" s="55"/>
+      <c r="BV30" s="55"/>
+      <c r="BW30" s="55"/>
+      <c r="BX30" s="55"/>
+      <c r="BY30" s="55"/>
+      <c r="BZ30" s="55"/>
+      <c r="CA30" s="55"/>
+      <c r="CB30" s="55"/>
+      <c r="CC30" s="55"/>
+      <c r="CD30" s="55"/>
+      <c r="CE30" s="55"/>
+      <c r="CF30" s="55"/>
+      <c r="CG30" s="55"/>
+      <c r="CH30" s="55"/>
+      <c r="CI30" s="55"/>
+      <c r="CJ30" s="55"/>
+      <c r="CK30" s="55"/>
+      <c r="CL30" s="55"/>
+      <c r="CM30" s="55"/>
+      <c r="CN30" s="55"/>
+      <c r="CO30" s="55"/>
+      <c r="CP30" s="55"/>
+      <c r="CQ30" s="55"/>
+      <c r="CR30" s="55"/>
+      <c r="CS30" s="55"/>
+      <c r="CT30" s="55"/>
+      <c r="CU30" s="55"/>
+      <c r="CV30" s="55"/>
+      <c r="CW30" s="55"/>
+      <c r="CX30" s="55"/>
+      <c r="CY30" s="55"/>
+      <c r="CZ30" s="55"/>
+      <c r="DA30" s="55"/>
+      <c r="DB30" s="55"/>
+      <c r="DC30" s="55"/>
+      <c r="DD30" s="55"/>
+      <c r="DE30" s="55"/>
+      <c r="DF30" s="55"/>
+      <c r="DG30" s="55"/>
+      <c r="DH30" s="55"/>
+      <c r="DI30" s="55"/>
+      <c r="DJ30" s="55"/>
+      <c r="DK30" s="55"/>
+      <c r="DL30" s="55"/>
+      <c r="DM30" s="55"/>
+      <c r="DN30" s="55"/>
+      <c r="DO30" s="55"/>
+      <c r="DP30" s="55"/>
+      <c r="DQ30" s="55"/>
+      <c r="DR30" s="55"/>
+      <c r="DS30" s="55"/>
+      <c r="DT30" s="55"/>
+      <c r="DU30" s="55"/>
+      <c r="DV30" s="55"/>
+      <c r="DW30" s="55"/>
+      <c r="DX30" s="55"/>
+      <c r="DY30" s="55"/>
+      <c r="DZ30" s="55"/>
+      <c r="EA30" s="55"/>
+      <c r="EB30" s="55"/>
+      <c r="EC30" s="55"/>
+      <c r="ED30" s="55"/>
+      <c r="EE30" s="55"/>
+      <c r="EF30" s="55"/>
+      <c r="EG30" s="55"/>
+      <c r="EH30" s="55"/>
+      <c r="EI30" s="55"/>
+      <c r="EJ30" s="55"/>
+      <c r="EK30" s="55"/>
+      <c r="EL30" s="55"/>
+      <c r="EM30" s="55"/>
+      <c r="EN30" s="55"/>
+      <c r="EO30" s="55"/>
+      <c r="EP30" s="55"/>
+      <c r="EQ30" s="55"/>
+      <c r="ER30" s="55"/>
+      <c r="ES30" s="55"/>
+      <c r="ET30" s="55"/>
+      <c r="EU30" s="55"/>
+      <c r="EV30" s="55"/>
+      <c r="EW30" s="55"/>
+      <c r="EX30" s="55"/>
+      <c r="EY30" s="55"/>
+      <c r="EZ30" s="55"/>
+      <c r="FA30" s="55"/>
+      <c r="FB30" s="55"/>
+      <c r="FC30" s="55"/>
+      <c r="FD30" s="55"/>
+      <c r="FE30" s="55"/>
+      <c r="FF30" s="55"/>
+      <c r="FG30" s="55"/>
+      <c r="FH30" s="55"/>
+      <c r="FI30" s="55"/>
+      <c r="FJ30" s="55"/>
+      <c r="FK30" s="55"/>
+      <c r="FL30" s="55"/>
+      <c r="FM30" s="55"/>
+      <c r="FN30" s="55"/>
+      <c r="FO30" s="55"/>
+      <c r="FP30" s="55"/>
+      <c r="FQ30" s="55"/>
+      <c r="FR30" s="55"/>
+      <c r="FS30" s="55"/>
+      <c r="FT30" s="55"/>
+      <c r="FU30" s="55"/>
+      <c r="FV30" s="55"/>
+      <c r="FW30" s="55"/>
+      <c r="FX30" s="55"/>
+      <c r="FY30" s="55"/>
+      <c r="FZ30" s="55"/>
+      <c r="GA30" s="55"/>
+      <c r="GB30" s="55"/>
+      <c r="GC30" s="55"/>
+      <c r="GD30" s="55"/>
+      <c r="GE30" s="55"/>
+      <c r="GF30" s="55"/>
+      <c r="GG30" s="55"/>
+      <c r="GH30" s="55"/>
+      <c r="GI30" s="55"/>
+      <c r="GJ30" s="55"/>
+      <c r="GK30" s="55"/>
+      <c r="GL30" s="55"/>
+      <c r="GM30" s="55"/>
+      <c r="GN30" s="55"/>
+      <c r="GO30" s="55"/>
+      <c r="GP30" s="55"/>
+      <c r="GQ30" s="55"/>
+      <c r="GR30" s="55"/>
+      <c r="GS30" s="55"/>
+      <c r="GT30" s="55"/>
+      <c r="GU30" s="55"/>
+      <c r="GV30" s="55"/>
+      <c r="GW30" s="55"/>
+      <c r="GX30" s="55"/>
+      <c r="GY30" s="55"/>
+      <c r="GZ30" s="55"/>
+      <c r="HA30" s="55"/>
+      <c r="HB30" s="55"/>
+      <c r="HC30" s="55"/>
+      <c r="HD30" s="55"/>
+      <c r="HE30" s="55"/>
+      <c r="HF30" s="55"/>
+      <c r="HG30" s="55"/>
+      <c r="HH30" s="55"/>
+      <c r="HI30" s="55"/>
+      <c r="HJ30" s="55"/>
+      <c r="HK30" s="55"/>
+      <c r="HL30" s="55"/>
+      <c r="HM30" s="55"/>
+      <c r="HN30" s="55"/>
+      <c r="HO30" s="55"/>
+      <c r="HP30" s="55"/>
+      <c r="HQ30" s="55"/>
+      <c r="HR30" s="55"/>
+      <c r="HS30" s="55"/>
+      <c r="HT30" s="55"/>
+      <c r="HU30" s="55"/>
+      <c r="HV30" s="55"/>
+      <c r="HW30" s="55"/>
+      <c r="HX30" s="55"/>
+      <c r="HY30" s="55"/>
+      <c r="HZ30" s="55"/>
+      <c r="IA30" s="55"/>
+      <c r="IB30" s="55"/>
+      <c r="IC30" s="55"/>
+      <c r="ID30" s="55"/>
+      <c r="IE30" s="55"/>
+      <c r="IF30" s="55"/>
+      <c r="IG30" s="55"/>
+      <c r="IH30" s="55"/>
+      <c r="II30" s="55"/>
+      <c r="IJ30" s="55"/>
+      <c r="IK30" s="55"/>
+      <c r="IL30" s="55"/>
+      <c r="IM30" s="55"/>
+      <c r="IN30" s="55"/>
+      <c r="IO30" s="55"/>
+      <c r="IP30" s="40"/>
       <c r="IQ30" s="14"/>
       <c r="IR30" s="14"/>
       <c r="IS30" s="14"/>
@@ -10319,22 +10319,22 @@
       <c r="IX30" s="14"/>
     </row>
     <row r="31" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="66" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="24">
-        <f>DATE(2021,11,15)</f>
-        <v>44515</v>
-      </c>
-      <c r="D31" s="24">
-        <f>DATE(2022,1,31)</f>
-        <v>44592</v>
+      <c r="A31" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="60"/>
+      <c r="C31" s="34">
+        <f>DATE(2022,1,23)</f>
+        <v>44584</v>
+      </c>
+      <c r="D31" s="34">
+        <f>DATE(2022,2,13)</f>
+        <v>44605</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="13">
         <f t="shared" si="156"/>
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
@@ -10350,235 +10350,235 @@
       <c r="R31" s="14"/>
       <c r="S31" s="14"/>
       <c r="T31" s="14"/>
-      <c r="U31" s="14"/>
-      <c r="V31" s="14"/>
-      <c r="W31" s="14"/>
-      <c r="X31" s="14"/>
-      <c r="Y31" s="14"/>
-      <c r="Z31" s="14"/>
-      <c r="AA31" s="14"/>
-      <c r="AB31" s="14"/>
-      <c r="AC31" s="14"/>
-      <c r="AD31" s="14"/>
-      <c r="AE31" s="14"/>
-      <c r="AF31" s="14"/>
-      <c r="AG31" s="14"/>
-      <c r="AH31" s="14"/>
-      <c r="AI31" s="14"/>
-      <c r="AJ31" s="14"/>
-      <c r="AK31" s="14"/>
-      <c r="AL31" s="14"/>
-      <c r="AM31" s="14"/>
-      <c r="AN31" s="14"/>
-      <c r="AO31" s="14"/>
-      <c r="AP31" s="14"/>
-      <c r="AQ31" s="14"/>
-      <c r="AR31" s="14"/>
-      <c r="AS31" s="14"/>
-      <c r="AT31" s="14"/>
-      <c r="AU31" s="14"/>
-      <c r="AV31" s="14"/>
-      <c r="AW31" s="14"/>
-      <c r="AX31" s="14"/>
-      <c r="AY31" s="14"/>
-      <c r="AZ31" s="14"/>
-      <c r="BA31" s="14"/>
-      <c r="BB31" s="14"/>
-      <c r="BC31" s="14"/>
-      <c r="BD31" s="14"/>
-      <c r="BE31" s="14"/>
-      <c r="BF31" s="14"/>
-      <c r="BG31" s="14"/>
-      <c r="BH31" s="14"/>
-      <c r="BI31" s="14"/>
-      <c r="BJ31" s="14"/>
-      <c r="BK31" s="14"/>
-      <c r="BL31" s="14"/>
-      <c r="BM31" s="14"/>
-      <c r="BN31" s="14"/>
-      <c r="BO31" s="14"/>
-      <c r="BP31" s="14"/>
-      <c r="BQ31" s="14"/>
-      <c r="BR31" s="14"/>
-      <c r="BS31" s="14"/>
-      <c r="BT31" s="14"/>
-      <c r="BU31" s="14"/>
-      <c r="BV31" s="14"/>
-      <c r="BW31" s="14"/>
-      <c r="BX31" s="14"/>
-      <c r="BY31" s="14"/>
-      <c r="BZ31" s="14"/>
-      <c r="CA31" s="14"/>
-      <c r="CB31" s="14"/>
-      <c r="CC31" s="14"/>
-      <c r="CD31" s="14"/>
-      <c r="CE31" s="14"/>
-      <c r="CF31" s="14"/>
-      <c r="CG31" s="14"/>
-      <c r="CH31" s="14"/>
-      <c r="CI31" s="14"/>
-      <c r="CJ31" s="14"/>
-      <c r="CK31" s="14"/>
-      <c r="CL31" s="14"/>
-      <c r="CM31" s="14"/>
-      <c r="CN31" s="14"/>
-      <c r="CO31" s="14"/>
-      <c r="CP31" s="14"/>
-      <c r="CQ31" s="14"/>
-      <c r="CR31" s="14"/>
-      <c r="CS31" s="14"/>
-      <c r="CT31" s="14"/>
-      <c r="CU31" s="14"/>
-      <c r="CV31" s="14"/>
-      <c r="CW31" s="14"/>
-      <c r="CX31" s="14"/>
-      <c r="CY31" s="14"/>
-      <c r="CZ31" s="14"/>
-      <c r="DA31" s="14"/>
-      <c r="DB31" s="14"/>
-      <c r="DC31" s="14"/>
-      <c r="DD31" s="14"/>
-      <c r="DE31" s="14"/>
-      <c r="DF31" s="14"/>
-      <c r="DG31" s="14"/>
-      <c r="DH31" s="14"/>
-      <c r="DI31" s="14"/>
-      <c r="DJ31" s="14"/>
-      <c r="DK31" s="14"/>
-      <c r="DL31" s="14"/>
-      <c r="DM31" s="14"/>
-      <c r="DN31" s="14"/>
-      <c r="DO31" s="14"/>
-      <c r="DP31" s="14"/>
-      <c r="DQ31" s="14"/>
-      <c r="DR31" s="14"/>
-      <c r="DS31" s="14"/>
-      <c r="DT31" s="14"/>
-      <c r="DU31" s="14"/>
-      <c r="DV31" s="14"/>
-      <c r="DW31" s="14"/>
-      <c r="DX31" s="14"/>
-      <c r="DY31" s="14"/>
-      <c r="DZ31" s="14"/>
-      <c r="EA31" s="14"/>
-      <c r="EB31" s="14"/>
-      <c r="EC31" s="14"/>
-      <c r="ED31" s="14"/>
-      <c r="EE31" s="14"/>
-      <c r="EF31" s="14"/>
-      <c r="EG31" s="14"/>
-      <c r="EH31" s="14"/>
-      <c r="EI31" s="14"/>
-      <c r="EJ31" s="14"/>
-      <c r="EK31" s="14"/>
-      <c r="EL31" s="14"/>
-      <c r="EM31" s="14"/>
-      <c r="EN31" s="14"/>
-      <c r="EO31" s="14"/>
-      <c r="EP31" s="14"/>
-      <c r="EQ31" s="14"/>
-      <c r="ER31" s="14"/>
-      <c r="ES31" s="14"/>
-      <c r="ET31" s="14"/>
-      <c r="EU31" s="14"/>
-      <c r="EV31" s="14"/>
-      <c r="EW31" s="14"/>
-      <c r="EX31" s="14"/>
-      <c r="EY31" s="14"/>
-      <c r="EZ31" s="14"/>
-      <c r="FA31" s="14"/>
-      <c r="FB31" s="14"/>
-      <c r="FC31" s="14"/>
-      <c r="FD31" s="14"/>
-      <c r="FE31" s="14"/>
-      <c r="FF31" s="14"/>
-      <c r="FG31" s="14"/>
-      <c r="FH31" s="14"/>
-      <c r="FI31" s="14"/>
-      <c r="FJ31" s="14"/>
-      <c r="FK31" s="14"/>
-      <c r="FL31" s="14"/>
-      <c r="FM31" s="14"/>
-      <c r="FN31" s="14"/>
-      <c r="FO31" s="14"/>
-      <c r="FP31" s="14"/>
-      <c r="FQ31" s="14"/>
-      <c r="FR31" s="14"/>
-      <c r="FS31" s="14"/>
-      <c r="FT31" s="14"/>
-      <c r="FU31" s="14"/>
-      <c r="FV31" s="14"/>
-      <c r="FW31" s="14"/>
-      <c r="FX31" s="14"/>
-      <c r="FY31" s="14"/>
-      <c r="FZ31" s="14"/>
-      <c r="GA31" s="14"/>
-      <c r="GB31" s="14"/>
-      <c r="GC31" s="14"/>
-      <c r="GD31" s="14"/>
-      <c r="GE31" s="14"/>
-      <c r="GF31" s="14"/>
-      <c r="GG31" s="14"/>
-      <c r="GH31" s="14"/>
-      <c r="GI31" s="14"/>
-      <c r="GJ31" s="14"/>
-      <c r="GK31" s="14"/>
-      <c r="GL31" s="14"/>
-      <c r="GM31" s="14"/>
-      <c r="GN31" s="14"/>
-      <c r="GO31" s="14"/>
-      <c r="GP31" s="14"/>
-      <c r="GQ31" s="14"/>
-      <c r="GR31" s="14"/>
-      <c r="GS31" s="14"/>
-      <c r="GT31" s="14"/>
-      <c r="GU31" s="14"/>
-      <c r="GV31" s="14"/>
-      <c r="GW31" s="14"/>
-      <c r="GX31" s="14"/>
-      <c r="GY31" s="14"/>
-      <c r="GZ31" s="14"/>
-      <c r="HA31" s="14"/>
-      <c r="HB31" s="14"/>
-      <c r="HC31" s="14"/>
-      <c r="HD31" s="14"/>
-      <c r="HE31" s="14"/>
-      <c r="HF31" s="14"/>
-      <c r="HG31" s="14"/>
-      <c r="HH31" s="14"/>
-      <c r="HI31" s="14"/>
-      <c r="HJ31" s="14"/>
-      <c r="HK31" s="14"/>
-      <c r="HL31" s="14"/>
-      <c r="HM31" s="14"/>
-      <c r="HN31" s="14"/>
-      <c r="HO31" s="14"/>
-      <c r="HP31" s="14"/>
-      <c r="HQ31" s="14"/>
-      <c r="HR31" s="14"/>
-      <c r="HS31" s="14"/>
-      <c r="HT31" s="14"/>
-      <c r="HU31" s="14"/>
-      <c r="HV31" s="14"/>
-      <c r="HW31" s="14"/>
-      <c r="HX31" s="14"/>
-      <c r="HY31" s="14"/>
-      <c r="HZ31" s="14"/>
-      <c r="IA31" s="14"/>
-      <c r="IB31" s="14"/>
-      <c r="IC31" s="14"/>
-      <c r="ID31" s="14"/>
-      <c r="IE31" s="14"/>
-      <c r="IF31" s="14"/>
-      <c r="IG31" s="14"/>
-      <c r="IH31" s="14"/>
-      <c r="II31" s="14"/>
-      <c r="IJ31" s="14"/>
-      <c r="IK31" s="14"/>
-      <c r="IL31" s="14"/>
-      <c r="IM31" s="14"/>
-      <c r="IN31" s="14"/>
-      <c r="IO31" s="14"/>
+      <c r="U31" s="42"/>
+      <c r="V31" s="42"/>
+      <c r="W31" s="42"/>
+      <c r="X31" s="42"/>
+      <c r="Y31" s="42"/>
+      <c r="Z31" s="42"/>
+      <c r="AA31" s="42"/>
+      <c r="AB31" s="42"/>
+      <c r="AC31" s="42"/>
+      <c r="AD31" s="42"/>
+      <c r="AE31" s="42"/>
+      <c r="AF31" s="42"/>
+      <c r="AG31" s="42"/>
+      <c r="AH31" s="42"/>
+      <c r="AI31" s="42"/>
+      <c r="AJ31" s="42"/>
+      <c r="AK31" s="42"/>
+      <c r="AL31" s="42"/>
+      <c r="AM31" s="42"/>
+      <c r="AN31" s="42"/>
+      <c r="AO31" s="42"/>
+      <c r="AP31" s="42"/>
+      <c r="AQ31" s="42"/>
+      <c r="AR31" s="42"/>
+      <c r="AS31" s="42"/>
+      <c r="AT31" s="42"/>
+      <c r="AU31" s="42"/>
+      <c r="AV31" s="42"/>
+      <c r="AW31" s="42"/>
+      <c r="AX31" s="42"/>
+      <c r="AY31" s="42"/>
+      <c r="AZ31" s="42"/>
+      <c r="BA31" s="42"/>
+      <c r="BB31" s="42"/>
+      <c r="BC31" s="42"/>
+      <c r="BD31" s="42"/>
+      <c r="BE31" s="42"/>
+      <c r="BF31" s="42"/>
+      <c r="BG31" s="42"/>
+      <c r="BH31" s="42"/>
+      <c r="BI31" s="42"/>
+      <c r="BJ31" s="42"/>
+      <c r="BK31" s="42"/>
+      <c r="BL31" s="42"/>
+      <c r="BM31" s="42"/>
+      <c r="BN31" s="42"/>
+      <c r="BO31" s="42"/>
+      <c r="BP31" s="42"/>
+      <c r="BQ31" s="42"/>
+      <c r="BR31" s="42"/>
+      <c r="BS31" s="42"/>
+      <c r="BT31" s="42"/>
+      <c r="BU31" s="42"/>
+      <c r="BV31" s="42"/>
+      <c r="BW31" s="42"/>
+      <c r="BX31" s="42"/>
+      <c r="BY31" s="42"/>
+      <c r="BZ31" s="42"/>
+      <c r="CA31" s="42"/>
+      <c r="CB31" s="42"/>
+      <c r="CC31" s="42"/>
+      <c r="CD31" s="42"/>
+      <c r="CE31" s="42"/>
+      <c r="CF31" s="42"/>
+      <c r="CG31" s="42"/>
+      <c r="CH31" s="42"/>
+      <c r="CI31" s="42"/>
+      <c r="CJ31" s="42"/>
+      <c r="CK31" s="42"/>
+      <c r="CL31" s="42"/>
+      <c r="CM31" s="42"/>
+      <c r="CN31" s="42"/>
+      <c r="CO31" s="42"/>
+      <c r="CP31" s="42"/>
+      <c r="CQ31" s="42"/>
+      <c r="CR31" s="42"/>
+      <c r="CS31" s="42"/>
+      <c r="CT31" s="42"/>
+      <c r="CU31" s="42"/>
+      <c r="CV31" s="42"/>
+      <c r="CW31" s="42"/>
+      <c r="CX31" s="42"/>
+      <c r="CY31" s="42"/>
+      <c r="CZ31" s="42"/>
+      <c r="DA31" s="42"/>
+      <c r="DB31" s="42"/>
+      <c r="DC31" s="42"/>
+      <c r="DD31" s="42"/>
+      <c r="DE31" s="42"/>
+      <c r="DF31" s="42"/>
+      <c r="DG31" s="42"/>
+      <c r="DH31" s="42"/>
+      <c r="DI31" s="42"/>
+      <c r="DJ31" s="42"/>
+      <c r="DK31" s="42"/>
+      <c r="DL31" s="42"/>
+      <c r="DM31" s="42"/>
+      <c r="DN31" s="42"/>
+      <c r="DO31" s="42"/>
+      <c r="DP31" s="42"/>
+      <c r="DQ31" s="42"/>
+      <c r="DR31" s="42"/>
+      <c r="DS31" s="42"/>
+      <c r="DT31" s="42"/>
+      <c r="DU31" s="42"/>
+      <c r="DV31" s="42"/>
+      <c r="DW31" s="42"/>
+      <c r="DX31" s="42"/>
+      <c r="DY31" s="42"/>
+      <c r="DZ31" s="42"/>
+      <c r="EA31" s="42"/>
+      <c r="EB31" s="42"/>
+      <c r="EC31" s="42"/>
+      <c r="ED31" s="42"/>
+      <c r="EE31" s="42"/>
+      <c r="EF31" s="42"/>
+      <c r="EG31" s="42"/>
+      <c r="EH31" s="42"/>
+      <c r="EI31" s="42"/>
+      <c r="EJ31" s="42"/>
+      <c r="EK31" s="42"/>
+      <c r="EL31" s="42"/>
+      <c r="EM31" s="42"/>
+      <c r="EN31" s="42"/>
+      <c r="EO31" s="42"/>
+      <c r="EP31" s="42"/>
+      <c r="EQ31" s="42"/>
+      <c r="ER31" s="42"/>
+      <c r="ES31" s="42"/>
+      <c r="ET31" s="42"/>
+      <c r="EU31" s="42"/>
+      <c r="EV31" s="42"/>
+      <c r="EW31" s="42"/>
+      <c r="EX31" s="42"/>
+      <c r="EY31" s="42"/>
+      <c r="EZ31" s="42"/>
+      <c r="FA31" s="42"/>
+      <c r="FB31" s="42"/>
+      <c r="FC31" s="42"/>
+      <c r="FD31" s="42"/>
+      <c r="FE31" s="42"/>
+      <c r="FF31" s="42"/>
+      <c r="FG31" s="42"/>
+      <c r="FH31" s="42"/>
+      <c r="FI31" s="42"/>
+      <c r="FJ31" s="42"/>
+      <c r="FK31" s="42"/>
+      <c r="FL31" s="42"/>
+      <c r="FM31" s="42"/>
+      <c r="FN31" s="42"/>
+      <c r="FO31" s="42"/>
+      <c r="FP31" s="42"/>
+      <c r="FQ31" s="42"/>
+      <c r="FR31" s="42"/>
+      <c r="FS31" s="42"/>
+      <c r="FT31" s="42"/>
+      <c r="FU31" s="42"/>
+      <c r="FV31" s="42"/>
+      <c r="FW31" s="42"/>
+      <c r="FX31" s="42"/>
+      <c r="FY31" s="42"/>
+      <c r="FZ31" s="42"/>
+      <c r="GA31" s="42"/>
+      <c r="GB31" s="42"/>
+      <c r="GC31" s="42"/>
+      <c r="GD31" s="42"/>
+      <c r="GE31" s="42"/>
+      <c r="GF31" s="42"/>
+      <c r="GG31" s="42"/>
+      <c r="GH31" s="42"/>
+      <c r="GI31" s="42"/>
+      <c r="GJ31" s="42"/>
+      <c r="GK31" s="42"/>
+      <c r="GL31" s="42"/>
+      <c r="GM31" s="42"/>
+      <c r="GN31" s="42"/>
+      <c r="GO31" s="42"/>
+      <c r="GP31" s="42"/>
+      <c r="GQ31" s="42"/>
+      <c r="GR31" s="42"/>
+      <c r="GS31" s="42"/>
+      <c r="GT31" s="42"/>
+      <c r="GU31" s="42"/>
+      <c r="GV31" s="42"/>
+      <c r="GW31" s="42"/>
+      <c r="GX31" s="42"/>
+      <c r="GY31" s="42"/>
+      <c r="GZ31" s="42"/>
+      <c r="HA31" s="42"/>
+      <c r="HB31" s="42"/>
+      <c r="HC31" s="42"/>
+      <c r="HD31" s="42"/>
+      <c r="HE31" s="42"/>
+      <c r="HF31" s="42"/>
+      <c r="HG31" s="42"/>
+      <c r="HH31" s="42"/>
+      <c r="HI31" s="42"/>
+      <c r="HJ31" s="42"/>
+      <c r="HK31" s="42"/>
+      <c r="HL31" s="42"/>
+      <c r="HM31" s="42"/>
+      <c r="HN31" s="42"/>
+      <c r="HO31" s="42"/>
+      <c r="HP31" s="42"/>
+      <c r="HQ31" s="42"/>
+      <c r="HR31" s="42"/>
+      <c r="HS31" s="42"/>
+      <c r="HT31" s="42"/>
+      <c r="HU31" s="42"/>
+      <c r="HV31" s="42"/>
+      <c r="HW31" s="42"/>
+      <c r="HX31" s="42"/>
+      <c r="HY31" s="42"/>
+      <c r="HZ31" s="42"/>
+      <c r="IA31" s="42"/>
+      <c r="IB31" s="42"/>
+      <c r="IC31" s="42"/>
+      <c r="ID31" s="42"/>
+      <c r="IE31" s="42"/>
+      <c r="IF31" s="42"/>
+      <c r="IG31" s="42"/>
+      <c r="IH31" s="42"/>
+      <c r="II31" s="42"/>
+      <c r="IJ31" s="42"/>
+      <c r="IK31" s="42"/>
+      <c r="IL31" s="42"/>
+      <c r="IM31" s="42"/>
+      <c r="IN31" s="42"/>
+      <c r="IO31" s="42"/>
       <c r="IP31" s="14"/>
       <c r="IQ31" s="14"/>
       <c r="IR31" s="14"/>
@@ -10590,22 +10590,22 @@
       <c r="IX31" s="14"/>
     </row>
     <row r="32" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="66"/>
+      <c r="A32" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="58"/>
       <c r="C32" s="24">
-        <f>DATE(2022,6,1)</f>
-        <v>44713</v>
+        <f>DATE(2021,11,15)</f>
+        <v>44515</v>
       </c>
       <c r="D32" s="24">
-        <f>DATE(2022,6,31)</f>
-        <v>44743</v>
+        <f>DATE(2022,1,31)</f>
+        <v>44592</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="13">
         <f t="shared" si="156"/>
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
@@ -10861,14 +10861,22 @@
       <c r="IX32" s="14"/>
     </row>
     <row r="33" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
+      <c r="A33" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="58"/>
+      <c r="C33" s="24">
+        <f>DATE(2022,6,1)</f>
+        <v>44713</v>
+      </c>
+      <c r="D33" s="24">
+        <f>DATE(2022,6,31)</f>
+        <v>44743</v>
+      </c>
       <c r="E33" s="13"/>
-      <c r="F33" s="13" t="str">
+      <c r="F33" s="13">
         <f t="shared" si="156"/>
-        <v/>
+        <v>31</v>
       </c>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
@@ -11123,39 +11131,291 @@
       <c r="IW33" s="14"/>
       <c r="IX33" s="14"/>
     </row>
-    <row r="34" spans="1:258" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E34" s="4"/>
+    <row r="34" spans="1:258" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13" t="str">
+        <f t="shared" si="156"/>
+        <v/>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="14"/>
+      <c r="U34" s="14"/>
+      <c r="V34" s="14"/>
+      <c r="W34" s="14"/>
+      <c r="X34" s="14"/>
+      <c r="Y34" s="14"/>
+      <c r="Z34" s="14"/>
+      <c r="AA34" s="14"/>
+      <c r="AB34" s="14"/>
+      <c r="AC34" s="14"/>
+      <c r="AD34" s="14"/>
+      <c r="AE34" s="14"/>
+      <c r="AF34" s="14"/>
+      <c r="AG34" s="14"/>
+      <c r="AH34" s="14"/>
+      <c r="AI34" s="14"/>
+      <c r="AJ34" s="14"/>
+      <c r="AK34" s="14"/>
+      <c r="AL34" s="14"/>
+      <c r="AM34" s="14"/>
+      <c r="AN34" s="14"/>
+      <c r="AO34" s="14"/>
+      <c r="AP34" s="14"/>
+      <c r="AQ34" s="14"/>
+      <c r="AR34" s="14"/>
+      <c r="AS34" s="14"/>
+      <c r="AT34" s="14"/>
+      <c r="AU34" s="14"/>
+      <c r="AV34" s="14"/>
+      <c r="AW34" s="14"/>
+      <c r="AX34" s="14"/>
+      <c r="AY34" s="14"/>
+      <c r="AZ34" s="14"/>
+      <c r="BA34" s="14"/>
+      <c r="BB34" s="14"/>
+      <c r="BC34" s="14"/>
+      <c r="BD34" s="14"/>
+      <c r="BE34" s="14"/>
+      <c r="BF34" s="14"/>
+      <c r="BG34" s="14"/>
+      <c r="BH34" s="14"/>
+      <c r="BI34" s="14"/>
+      <c r="BJ34" s="14"/>
+      <c r="BK34" s="14"/>
+      <c r="BL34" s="14"/>
+      <c r="BM34" s="14"/>
+      <c r="BN34" s="14"/>
+      <c r="BO34" s="14"/>
+      <c r="BP34" s="14"/>
+      <c r="BQ34" s="14"/>
+      <c r="BR34" s="14"/>
+      <c r="BS34" s="14"/>
+      <c r="BT34" s="14"/>
+      <c r="BU34" s="14"/>
+      <c r="BV34" s="14"/>
+      <c r="BW34" s="14"/>
+      <c r="BX34" s="14"/>
+      <c r="BY34" s="14"/>
+      <c r="BZ34" s="14"/>
+      <c r="CA34" s="14"/>
+      <c r="CB34" s="14"/>
+      <c r="CC34" s="14"/>
+      <c r="CD34" s="14"/>
+      <c r="CE34" s="14"/>
+      <c r="CF34" s="14"/>
+      <c r="CG34" s="14"/>
+      <c r="CH34" s="14"/>
+      <c r="CI34" s="14"/>
+      <c r="CJ34" s="14"/>
+      <c r="CK34" s="14"/>
+      <c r="CL34" s="14"/>
+      <c r="CM34" s="14"/>
+      <c r="CN34" s="14"/>
+      <c r="CO34" s="14"/>
+      <c r="CP34" s="14"/>
+      <c r="CQ34" s="14"/>
+      <c r="CR34" s="14"/>
+      <c r="CS34" s="14"/>
+      <c r="CT34" s="14"/>
+      <c r="CU34" s="14"/>
+      <c r="CV34" s="14"/>
+      <c r="CW34" s="14"/>
+      <c r="CX34" s="14"/>
+      <c r="CY34" s="14"/>
+      <c r="CZ34" s="14"/>
+      <c r="DA34" s="14"/>
+      <c r="DB34" s="14"/>
+      <c r="DC34" s="14"/>
+      <c r="DD34" s="14"/>
+      <c r="DE34" s="14"/>
+      <c r="DF34" s="14"/>
+      <c r="DG34" s="14"/>
+      <c r="DH34" s="14"/>
+      <c r="DI34" s="14"/>
+      <c r="DJ34" s="14"/>
+      <c r="DK34" s="14"/>
+      <c r="DL34" s="14"/>
+      <c r="DM34" s="14"/>
+      <c r="DN34" s="14"/>
+      <c r="DO34" s="14"/>
+      <c r="DP34" s="14"/>
+      <c r="DQ34" s="14"/>
+      <c r="DR34" s="14"/>
+      <c r="DS34" s="14"/>
+      <c r="DT34" s="14"/>
+      <c r="DU34" s="14"/>
+      <c r="DV34" s="14"/>
+      <c r="DW34" s="14"/>
+      <c r="DX34" s="14"/>
+      <c r="DY34" s="14"/>
+      <c r="DZ34" s="14"/>
+      <c r="EA34" s="14"/>
+      <c r="EB34" s="14"/>
+      <c r="EC34" s="14"/>
+      <c r="ED34" s="14"/>
+      <c r="EE34" s="14"/>
+      <c r="EF34" s="14"/>
+      <c r="EG34" s="14"/>
+      <c r="EH34" s="14"/>
+      <c r="EI34" s="14"/>
+      <c r="EJ34" s="14"/>
+      <c r="EK34" s="14"/>
+      <c r="EL34" s="14"/>
+      <c r="EM34" s="14"/>
+      <c r="EN34" s="14"/>
+      <c r="EO34" s="14"/>
+      <c r="EP34" s="14"/>
+      <c r="EQ34" s="14"/>
+      <c r="ER34" s="14"/>
+      <c r="ES34" s="14"/>
+      <c r="ET34" s="14"/>
+      <c r="EU34" s="14"/>
+      <c r="EV34" s="14"/>
+      <c r="EW34" s="14"/>
+      <c r="EX34" s="14"/>
+      <c r="EY34" s="14"/>
+      <c r="EZ34" s="14"/>
+      <c r="FA34" s="14"/>
+      <c r="FB34" s="14"/>
+      <c r="FC34" s="14"/>
+      <c r="FD34" s="14"/>
+      <c r="FE34" s="14"/>
+      <c r="FF34" s="14"/>
+      <c r="FG34" s="14"/>
+      <c r="FH34" s="14"/>
+      <c r="FI34" s="14"/>
+      <c r="FJ34" s="14"/>
+      <c r="FK34" s="14"/>
+      <c r="FL34" s="14"/>
+      <c r="FM34" s="14"/>
+      <c r="FN34" s="14"/>
+      <c r="FO34" s="14"/>
+      <c r="FP34" s="14"/>
+      <c r="FQ34" s="14"/>
+      <c r="FR34" s="14"/>
+      <c r="FS34" s="14"/>
+      <c r="FT34" s="14"/>
+      <c r="FU34" s="14"/>
+      <c r="FV34" s="14"/>
+      <c r="FW34" s="14"/>
+      <c r="FX34" s="14"/>
+      <c r="FY34" s="14"/>
+      <c r="FZ34" s="14"/>
+      <c r="GA34" s="14"/>
+      <c r="GB34" s="14"/>
+      <c r="GC34" s="14"/>
+      <c r="GD34" s="14"/>
+      <c r="GE34" s="14"/>
+      <c r="GF34" s="14"/>
+      <c r="GG34" s="14"/>
+      <c r="GH34" s="14"/>
+      <c r="GI34" s="14"/>
+      <c r="GJ34" s="14"/>
+      <c r="GK34" s="14"/>
+      <c r="GL34" s="14"/>
+      <c r="GM34" s="14"/>
+      <c r="GN34" s="14"/>
+      <c r="GO34" s="14"/>
+      <c r="GP34" s="14"/>
+      <c r="GQ34" s="14"/>
+      <c r="GR34" s="14"/>
+      <c r="GS34" s="14"/>
+      <c r="GT34" s="14"/>
+      <c r="GU34" s="14"/>
+      <c r="GV34" s="14"/>
+      <c r="GW34" s="14"/>
+      <c r="GX34" s="14"/>
+      <c r="GY34" s="14"/>
+      <c r="GZ34" s="14"/>
+      <c r="HA34" s="14"/>
+      <c r="HB34" s="14"/>
+      <c r="HC34" s="14"/>
+      <c r="HD34" s="14"/>
+      <c r="HE34" s="14"/>
+      <c r="HF34" s="14"/>
+      <c r="HG34" s="14"/>
+      <c r="HH34" s="14"/>
+      <c r="HI34" s="14"/>
+      <c r="HJ34" s="14"/>
+      <c r="HK34" s="14"/>
+      <c r="HL34" s="14"/>
+      <c r="HM34" s="14"/>
+      <c r="HN34" s="14"/>
+      <c r="HO34" s="14"/>
+      <c r="HP34" s="14"/>
+      <c r="HQ34" s="14"/>
+      <c r="HR34" s="14"/>
+      <c r="HS34" s="14"/>
+      <c r="HT34" s="14"/>
+      <c r="HU34" s="14"/>
+      <c r="HV34" s="14"/>
+      <c r="HW34" s="14"/>
+      <c r="HX34" s="14"/>
+      <c r="HY34" s="14"/>
+      <c r="HZ34" s="14"/>
+      <c r="IA34" s="14"/>
+      <c r="IB34" s="14"/>
+      <c r="IC34" s="14"/>
+      <c r="ID34" s="14"/>
+      <c r="IE34" s="14"/>
+      <c r="IF34" s="14"/>
+      <c r="IG34" s="14"/>
+      <c r="IH34" s="14"/>
+      <c r="II34" s="14"/>
+      <c r="IJ34" s="14"/>
+      <c r="IK34" s="14"/>
+      <c r="IL34" s="14"/>
+      <c r="IM34" s="14"/>
+      <c r="IN34" s="14"/>
+      <c r="IO34" s="14"/>
+      <c r="IP34" s="14"/>
+      <c r="IQ34" s="14"/>
+      <c r="IR34" s="14"/>
+      <c r="IS34" s="14"/>
+      <c r="IT34" s="14"/>
+      <c r="IU34" s="14"/>
+      <c r="IV34" s="14"/>
+      <c r="IW34" s="14"/>
+      <c r="IX34" s="14"/>
     </row>
     <row r="35" spans="1:258" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="16"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:258" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="EQ4:EW4"/>
-    <mergeCell ref="EX4:FD4"/>
-    <mergeCell ref="HW4:IC4"/>
-    <mergeCell ref="FE4:FK4"/>
-    <mergeCell ref="FL4:FR4"/>
-    <mergeCell ref="FS4:FY4"/>
-    <mergeCell ref="FZ4:GF4"/>
-    <mergeCell ref="GG4:GM4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="N4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="AB4:AH4"/>
+    <mergeCell ref="BK4:BQ4"/>
+    <mergeCell ref="BR4:BX4"/>
+    <mergeCell ref="BY4:CE4"/>
+    <mergeCell ref="CF4:CL4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="AI4:AO4"/>
+    <mergeCell ref="AP4:AV4"/>
+    <mergeCell ref="AW4:BC4"/>
+    <mergeCell ref="BD4:BJ4"/>
     <mergeCell ref="CM4:CS4"/>
     <mergeCell ref="ID4:IJ4"/>
     <mergeCell ref="IK4:IQ4"/>
@@ -11172,28 +11432,39 @@
     <mergeCell ref="DV4:EB4"/>
     <mergeCell ref="EC4:EI4"/>
     <mergeCell ref="EJ4:EP4"/>
-    <mergeCell ref="BK4:BQ4"/>
-    <mergeCell ref="BR4:BX4"/>
-    <mergeCell ref="BY4:CE4"/>
-    <mergeCell ref="CF4:CL4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="AI4:AO4"/>
-    <mergeCell ref="AP4:AV4"/>
-    <mergeCell ref="AW4:BC4"/>
-    <mergeCell ref="BD4:BJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="N4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="AB4:AH4"/>
+    <mergeCell ref="EQ4:EW4"/>
+    <mergeCell ref="EX4:FD4"/>
+    <mergeCell ref="HW4:IC4"/>
+    <mergeCell ref="FE4:FK4"/>
+    <mergeCell ref="FL4:FR4"/>
+    <mergeCell ref="FS4:FY4"/>
+    <mergeCell ref="FZ4:GF4"/>
+    <mergeCell ref="GG4:GM4"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A29:B29"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="G5:IX33">
+  <conditionalFormatting sqref="G5:IX34">
     <cfRule type="expression" dxfId="2" priority="126">
       <formula>AND(TODAY()&gt;=G$5,TODAY()&lt;H$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:IX33">
+  <conditionalFormatting sqref="G7:IX34">
     <cfRule type="expression" dxfId="1" priority="120">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
@@ -11327,6 +11598,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010021CB413651170D4FBFA874F8BEE755CA" ma:contentTypeVersion="7" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="42743fc73206d53d9dc0a38c59eadd60">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dc598aa0-d9ce-4a6b-81d3-1bfd1d95be93" xmlns:ns4="0f3824ba-70ce-4e7b-b9df-d016a901c15a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fe924b3eb92af8fdbe5696825ae74dba" ns3:_="" ns4:_="">
     <xsd:import namespace="dc598aa0-d9ce-4a6b-81d3-1bfd1d95be93"/>
@@ -11511,22 +11797,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B94DE01B-F382-4B59-8124-92C815CDB8D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA5933DF-E5C2-4102-897C-E72E9DA32B8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFF8F1F2-15C5-48DC-909D-47DBCB39B9F0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11543,21 +11831,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA5933DF-E5C2-4102-897C-E72E9DA32B8D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B94DE01B-F382-4B59-8124-92C815CDB8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>